<commit_message>
Atualizado por script em 07-11-2023 20:45
</commit_message>
<xml_diff>
--- a/2023/england_league-one_2023-2024.xlsx
+++ b/2023/england_league-one_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V182"/>
+  <dimension ref="A1:V184"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9313,71 +9313,71 @@
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>Bolton</t>
+          <t>Bristol Rovers</t>
         </is>
       </c>
       <c r="G97" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>Peterborough</t>
+          <t>Wigan</t>
         </is>
       </c>
       <c r="I97" t="n">
         <v>1</v>
       </c>
       <c r="J97" t="n">
-        <v>1.98</v>
+        <v>2.21</v>
       </c>
       <c r="K97" t="inlineStr">
         <is>
-          <t>19/09/2023 20:12</t>
+          <t>19/09/2023 16:12</t>
         </is>
       </c>
       <c r="L97" t="n">
-        <v>2.17</v>
+        <v>2.23</v>
       </c>
       <c r="M97" t="inlineStr">
         <is>
-          <t>23/09/2023 15:54</t>
+          <t>23/09/2023 15:48</t>
         </is>
       </c>
       <c r="N97" t="n">
-        <v>3.59</v>
+        <v>3.46</v>
       </c>
       <c r="O97" t="inlineStr">
         <is>
-          <t>19/09/2023 20:12</t>
+          <t>19/09/2023 16:12</t>
         </is>
       </c>
       <c r="P97" t="n">
-        <v>3.61</v>
+        <v>3.6</v>
       </c>
       <c r="Q97" t="inlineStr">
         <is>
-          <t>23/09/2023 15:54</t>
+          <t>23/09/2023 15:37</t>
         </is>
       </c>
       <c r="R97" t="n">
-        <v>3.84</v>
+        <v>3.14</v>
       </c>
       <c r="S97" t="inlineStr">
         <is>
-          <t>19/09/2023 20:12</t>
+          <t>19/09/2023 16:12</t>
         </is>
       </c>
       <c r="T97" t="n">
-        <v>3.39</v>
+        <v>3.26</v>
       </c>
       <c r="U97" t="inlineStr">
         <is>
-          <t>23/09/2023 15:54</t>
+          <t>23/09/2023 15:48</t>
         </is>
       </c>
       <c r="V97" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/bolton-peterborough/WtY5sZSp/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/bristol-rovers-wigan/WYws6I5o/</t>
         </is>
       </c>
     </row>
@@ -9497,71 +9497,71 @@
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>Blackpool</t>
+          <t>Burton</t>
         </is>
       </c>
       <c r="G99" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>Reading</t>
+          <t>Fleetwood</t>
         </is>
       </c>
       <c r="I99" t="n">
         <v>1</v>
       </c>
       <c r="J99" t="n">
-        <v>1.92</v>
+        <v>2.2</v>
       </c>
       <c r="K99" t="inlineStr">
         <is>
-          <t>19/09/2023 16:12</t>
+          <t>19/09/2023 20:12</t>
         </is>
       </c>
       <c r="L99" t="n">
-        <v>2.03</v>
+        <v>2.81</v>
       </c>
       <c r="M99" t="inlineStr">
         <is>
-          <t>23/09/2023 15:58</t>
+          <t>23/09/2023 15:37</t>
         </is>
       </c>
       <c r="N99" t="n">
-        <v>3.56</v>
+        <v>3.41</v>
       </c>
       <c r="O99" t="inlineStr">
         <is>
-          <t>19/09/2023 16:12</t>
+          <t>19/09/2023 20:12</t>
         </is>
       </c>
       <c r="P99" t="n">
-        <v>3.6</v>
+        <v>3.44</v>
       </c>
       <c r="Q99" t="inlineStr">
         <is>
-          <t>23/09/2023 15:58</t>
+          <t>23/09/2023 15:46</t>
         </is>
       </c>
       <c r="R99" t="n">
-        <v>4.13</v>
+        <v>3.38</v>
       </c>
       <c r="S99" t="inlineStr">
         <is>
-          <t>19/09/2023 16:12</t>
+          <t>19/09/2023 20:12</t>
         </is>
       </c>
       <c r="T99" t="n">
-        <v>3.79</v>
+        <v>2.58</v>
       </c>
       <c r="U99" t="inlineStr">
         <is>
-          <t>23/09/2023 15:58</t>
+          <t>23/09/2023 15:46</t>
         </is>
       </c>
       <c r="V99" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/blackpool-reading/fHAxa1bI/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/burton-fleetwood-town/APxo5xLi/</t>
         </is>
       </c>
     </row>
@@ -9681,7 +9681,7 @@
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>Burton</t>
+          <t>Bolton</t>
         </is>
       </c>
       <c r="G101" t="n">
@@ -9689,14 +9689,14 @@
       </c>
       <c r="H101" t="inlineStr">
         <is>
-          <t>Fleetwood</t>
+          <t>Peterborough</t>
         </is>
       </c>
       <c r="I101" t="n">
         <v>1</v>
       </c>
       <c r="J101" t="n">
-        <v>2.2</v>
+        <v>1.98</v>
       </c>
       <c r="K101" t="inlineStr">
         <is>
@@ -9704,15 +9704,15 @@
         </is>
       </c>
       <c r="L101" t="n">
-        <v>2.81</v>
+        <v>2.17</v>
       </c>
       <c r="M101" t="inlineStr">
         <is>
-          <t>23/09/2023 15:37</t>
+          <t>23/09/2023 15:54</t>
         </is>
       </c>
       <c r="N101" t="n">
-        <v>3.41</v>
+        <v>3.59</v>
       </c>
       <c r="O101" t="inlineStr">
         <is>
@@ -9720,15 +9720,15 @@
         </is>
       </c>
       <c r="P101" t="n">
-        <v>3.44</v>
+        <v>3.61</v>
       </c>
       <c r="Q101" t="inlineStr">
         <is>
-          <t>23/09/2023 15:46</t>
+          <t>23/09/2023 15:54</t>
         </is>
       </c>
       <c r="R101" t="n">
-        <v>3.38</v>
+        <v>3.84</v>
       </c>
       <c r="S101" t="inlineStr">
         <is>
@@ -9736,16 +9736,16 @@
         </is>
       </c>
       <c r="T101" t="n">
-        <v>2.58</v>
+        <v>3.39</v>
       </c>
       <c r="U101" t="inlineStr">
         <is>
-          <t>23/09/2023 15:46</t>
+          <t>23/09/2023 15:54</t>
         </is>
       </c>
       <c r="V101" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/burton-fleetwood-town/APxo5xLi/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/bolton-peterborough/WtY5sZSp/</t>
         </is>
       </c>
     </row>
@@ -9773,7 +9773,7 @@
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>Bristol Rovers</t>
+          <t>Blackpool</t>
         </is>
       </c>
       <c r="G102" t="n">
@@ -9781,14 +9781,14 @@
       </c>
       <c r="H102" t="inlineStr">
         <is>
-          <t>Wigan</t>
+          <t>Reading</t>
         </is>
       </c>
       <c r="I102" t="n">
         <v>1</v>
       </c>
       <c r="J102" t="n">
-        <v>2.21</v>
+        <v>1.92</v>
       </c>
       <c r="K102" t="inlineStr">
         <is>
@@ -9796,15 +9796,15 @@
         </is>
       </c>
       <c r="L102" t="n">
-        <v>2.23</v>
+        <v>2.03</v>
       </c>
       <c r="M102" t="inlineStr">
         <is>
-          <t>23/09/2023 15:48</t>
+          <t>23/09/2023 15:58</t>
         </is>
       </c>
       <c r="N102" t="n">
-        <v>3.46</v>
+        <v>3.56</v>
       </c>
       <c r="O102" t="inlineStr">
         <is>
@@ -9816,11 +9816,11 @@
       </c>
       <c r="Q102" t="inlineStr">
         <is>
-          <t>23/09/2023 15:37</t>
+          <t>23/09/2023 15:58</t>
         </is>
       </c>
       <c r="R102" t="n">
-        <v>3.14</v>
+        <v>4.13</v>
       </c>
       <c r="S102" t="inlineStr">
         <is>
@@ -9828,16 +9828,16 @@
         </is>
       </c>
       <c r="T102" t="n">
-        <v>3.26</v>
+        <v>3.79</v>
       </c>
       <c r="U102" t="inlineStr">
         <is>
-          <t>23/09/2023 15:48</t>
+          <t>23/09/2023 15:58</t>
         </is>
       </c>
       <c r="V102" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/bristol-rovers-wigan/WYws6I5o/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/blackpool-reading/fHAxa1bI/</t>
         </is>
       </c>
     </row>
@@ -9865,22 +9865,22 @@
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>Reading</t>
+          <t>Wycombe</t>
         </is>
       </c>
       <c r="G103" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H103" t="inlineStr">
         <is>
-          <t>Burton</t>
+          <t>Carlisle</t>
         </is>
       </c>
       <c r="I103" t="n">
         <v>0</v>
       </c>
       <c r="J103" t="n">
-        <v>2</v>
+        <v>1.78</v>
       </c>
       <c r="K103" t="inlineStr">
         <is>
@@ -9888,15 +9888,15 @@
         </is>
       </c>
       <c r="L103" t="n">
-        <v>1.92</v>
+        <v>1.96</v>
       </c>
       <c r="M103" t="inlineStr">
         <is>
-          <t>30/09/2023 15:57</t>
+          <t>30/09/2023 15:51</t>
         </is>
       </c>
       <c r="N103" t="n">
-        <v>3.32</v>
+        <v>3.7</v>
       </c>
       <c r="O103" t="inlineStr">
         <is>
@@ -9904,15 +9904,15 @@
         </is>
       </c>
       <c r="P103" t="n">
-        <v>3.8</v>
+        <v>3.41</v>
       </c>
       <c r="Q103" t="inlineStr">
         <is>
-          <t>30/09/2023 15:57</t>
+          <t>30/09/2023 15:51</t>
         </is>
       </c>
       <c r="R103" t="n">
-        <v>3.82</v>
+        <v>4.31</v>
       </c>
       <c r="S103" t="inlineStr">
         <is>
@@ -9920,16 +9920,16 @@
         </is>
       </c>
       <c r="T103" t="n">
-        <v>4</v>
+        <v>4.31</v>
       </c>
       <c r="U103" t="inlineStr">
         <is>
-          <t>30/09/2023 15:57</t>
+          <t>30/09/2023 15:51</t>
         </is>
       </c>
       <c r="V103" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/reading-burton/WGlF8BRq/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/wycombe-carlisle/YuV9Uhl3/</t>
         </is>
       </c>
     </row>
@@ -9957,22 +9957,22 @@
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>Barnsley</t>
+          <t>Wigan</t>
         </is>
       </c>
       <c r="G104" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H104" t="inlineStr">
         <is>
-          <t>Blackpool</t>
+          <t>Portsmouth</t>
         </is>
       </c>
       <c r="I104" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J104" t="n">
-        <v>2.18</v>
+        <v>3.14</v>
       </c>
       <c r="K104" t="inlineStr">
         <is>
@@ -9980,15 +9980,15 @@
         </is>
       </c>
       <c r="L104" t="n">
-        <v>2.51</v>
+        <v>3.11</v>
       </c>
       <c r="M104" t="inlineStr">
         <is>
-          <t>30/09/2023 15:50</t>
+          <t>30/09/2023 14:21</t>
         </is>
       </c>
       <c r="N104" t="n">
-        <v>3.31</v>
+        <v>3.21</v>
       </c>
       <c r="O104" t="inlineStr">
         <is>
@@ -9996,15 +9996,15 @@
         </is>
       </c>
       <c r="P104" t="n">
-        <v>3.6</v>
+        <v>3.59</v>
       </c>
       <c r="Q104" t="inlineStr">
         <is>
-          <t>30/09/2023 15:50</t>
+          <t>30/09/2023 15:38</t>
         </is>
       </c>
       <c r="R104" t="n">
-        <v>3.55</v>
+        <v>2.42</v>
       </c>
       <c r="S104" t="inlineStr">
         <is>
@@ -10012,16 +10012,16 @@
         </is>
       </c>
       <c r="T104" t="n">
-        <v>2.81</v>
+        <v>2.31</v>
       </c>
       <c r="U104" t="inlineStr">
         <is>
-          <t>30/09/2023 15:51</t>
+          <t>30/09/2023 14:21</t>
         </is>
       </c>
       <c r="V104" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/barnsley-blackpool/40HNIeki/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/wigan-portsmouth/KxR5VYYd/</t>
         </is>
       </c>
     </row>
@@ -10049,71 +10049,71 @@
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>Derby</t>
+          <t>Stevenage</t>
         </is>
       </c>
       <c r="G105" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H105" t="inlineStr">
         <is>
-          <t>Cambridge Utd</t>
+          <t>Oxford Utd</t>
         </is>
       </c>
       <c r="I105" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J105" t="n">
-        <v>1.56</v>
+        <v>2.53</v>
       </c>
       <c r="K105" t="inlineStr">
         <is>
-          <t>23/09/2023 17:13</t>
+          <t>24/09/2023 03:13</t>
         </is>
       </c>
       <c r="L105" t="n">
-        <v>1.64</v>
+        <v>2.42</v>
       </c>
       <c r="M105" t="inlineStr">
         <is>
-          <t>30/09/2023 15:58</t>
+          <t>30/09/2023 15:51</t>
         </is>
       </c>
       <c r="N105" t="n">
-        <v>4.18</v>
+        <v>3.2</v>
       </c>
       <c r="O105" t="inlineStr">
         <is>
-          <t>23/09/2023 17:13</t>
+          <t>24/09/2023 03:13</t>
         </is>
       </c>
       <c r="P105" t="n">
-        <v>4.2</v>
+        <v>3.42</v>
       </c>
       <c r="Q105" t="inlineStr">
         <is>
-          <t>30/09/2023 15:58</t>
+          <t>30/09/2023 15:51</t>
         </is>
       </c>
       <c r="R105" t="n">
-        <v>5.3</v>
+        <v>2.83</v>
       </c>
       <c r="S105" t="inlineStr">
         <is>
-          <t>23/09/2023 17:13</t>
+          <t>24/09/2023 03:13</t>
         </is>
       </c>
       <c r="T105" t="n">
-        <v>5.29</v>
+        <v>3.06</v>
       </c>
       <c r="U105" t="inlineStr">
         <is>
-          <t>30/09/2023 15:58</t>
+          <t>30/09/2023 15:51</t>
         </is>
       </c>
       <c r="V105" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/derby-cambridge-utd/riGRHF4c/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/stevenage-oxford-utd/IXnN6kdd/</t>
         </is>
       </c>
     </row>
@@ -10141,7 +10141,7 @@
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>Exeter</t>
+          <t>Shrewsbury</t>
         </is>
       </c>
       <c r="G106" t="n">
@@ -10149,63 +10149,63 @@
       </c>
       <c r="H106" t="inlineStr">
         <is>
-          <t>Northampton</t>
+          <t>Charlton</t>
         </is>
       </c>
       <c r="I106" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J106" t="n">
-        <v>1.73</v>
+        <v>2.67</v>
       </c>
       <c r="K106" t="inlineStr">
         <is>
-          <t>24/09/2023 03:13</t>
+          <t>23/09/2023 17:13</t>
         </is>
       </c>
       <c r="L106" t="n">
-        <v>2.13</v>
+        <v>3.08</v>
       </c>
       <c r="M106" t="inlineStr">
         <is>
-          <t>30/09/2023 15:51</t>
+          <t>30/09/2023 15:57</t>
         </is>
       </c>
       <c r="N106" t="n">
-        <v>3.48</v>
+        <v>3.15</v>
       </c>
       <c r="O106" t="inlineStr">
         <is>
-          <t>24/09/2023 03:13</t>
+          <t>23/09/2023 17:13</t>
         </is>
       </c>
       <c r="P106" t="n">
-        <v>3.53</v>
+        <v>3.43</v>
       </c>
       <c r="Q106" t="inlineStr">
         <is>
-          <t>30/09/2023 15:51</t>
+          <t>30/09/2023 15:18</t>
         </is>
       </c>
       <c r="R106" t="n">
-        <v>5.01</v>
+        <v>2.71</v>
       </c>
       <c r="S106" t="inlineStr">
         <is>
-          <t>24/09/2023 03:13</t>
+          <t>23/09/2023 17:13</t>
         </is>
       </c>
       <c r="T106" t="n">
-        <v>3.57</v>
+        <v>2.4</v>
       </c>
       <c r="U106" t="inlineStr">
         <is>
-          <t>30/09/2023 15:51</t>
+          <t>30/09/2023 15:57</t>
         </is>
       </c>
       <c r="V106" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/exeter-northampton/0SAWGZJ3/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/shrewsbury-charlton/vslJ7Vtj/</t>
         </is>
       </c>
     </row>
@@ -10233,22 +10233,22 @@
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>Fleetwood</t>
+          <t>Reading</t>
         </is>
       </c>
       <c r="G107" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H107" t="inlineStr">
         <is>
-          <t>Leyton Orient</t>
+          <t>Burton</t>
         </is>
       </c>
       <c r="I107" t="n">
         <v>0</v>
       </c>
       <c r="J107" t="n">
-        <v>2.16</v>
+        <v>2</v>
       </c>
       <c r="K107" t="inlineStr">
         <is>
@@ -10256,15 +10256,15 @@
         </is>
       </c>
       <c r="L107" t="n">
-        <v>2.23</v>
+        <v>1.92</v>
       </c>
       <c r="M107" t="inlineStr">
         <is>
-          <t>30/09/2023 15:50</t>
+          <t>30/09/2023 15:57</t>
         </is>
       </c>
       <c r="N107" t="n">
-        <v>3.36</v>
+        <v>3.32</v>
       </c>
       <c r="O107" t="inlineStr">
         <is>
@@ -10272,15 +10272,15 @@
         </is>
       </c>
       <c r="P107" t="n">
-        <v>3.48</v>
+        <v>3.8</v>
       </c>
       <c r="Q107" t="inlineStr">
         <is>
-          <t>30/09/2023 15:50</t>
+          <t>30/09/2023 15:57</t>
         </is>
       </c>
       <c r="R107" t="n">
-        <v>3.34</v>
+        <v>3.82</v>
       </c>
       <c r="S107" t="inlineStr">
         <is>
@@ -10288,16 +10288,16 @@
         </is>
       </c>
       <c r="T107" t="n">
-        <v>3.36</v>
+        <v>4</v>
       </c>
       <c r="U107" t="inlineStr">
         <is>
-          <t>30/09/2023 15:50</t>
+          <t>30/09/2023 15:57</t>
         </is>
       </c>
       <c r="V107" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/fleetwood-town-leyton-orient/vJ9zGgZ9/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/reading-burton/WGlF8BRq/</t>
         </is>
       </c>
     </row>
@@ -10325,22 +10325,22 @@
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>Lincoln</t>
+          <t>Port Vale</t>
         </is>
       </c>
       <c r="G108" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H108" t="inlineStr">
         <is>
-          <t>Cheltenham</t>
+          <t>Bolton</t>
         </is>
       </c>
       <c r="I108" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J108" t="n">
-        <v>1.81</v>
+        <v>3.09</v>
       </c>
       <c r="K108" t="inlineStr">
         <is>
@@ -10348,15 +10348,15 @@
         </is>
       </c>
       <c r="L108" t="n">
-        <v>1.76</v>
+        <v>2.64</v>
       </c>
       <c r="M108" t="inlineStr">
         <is>
-          <t>30/09/2023 15:39</t>
+          <t>30/09/2023 15:48</t>
         </is>
       </c>
       <c r="N108" t="n">
-        <v>3.55</v>
+        <v>3.23</v>
       </c>
       <c r="O108" t="inlineStr">
         <is>
@@ -10364,7 +10364,7 @@
         </is>
       </c>
       <c r="P108" t="n">
-        <v>3.7</v>
+        <v>3.49</v>
       </c>
       <c r="Q108" t="inlineStr">
         <is>
@@ -10372,7 +10372,7 @@
         </is>
       </c>
       <c r="R108" t="n">
-        <v>4.74</v>
+        <v>2.44</v>
       </c>
       <c r="S108" t="inlineStr">
         <is>
@@ -10380,16 +10380,16 @@
         </is>
       </c>
       <c r="T108" t="n">
-        <v>5.02</v>
+        <v>2.72</v>
       </c>
       <c r="U108" t="inlineStr">
         <is>
-          <t>30/09/2023 15:40</t>
+          <t>30/09/2023 15:48</t>
         </is>
       </c>
       <c r="V108" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/lincoln-city-cheltenham/Yu9vFDlG/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/port-vale-bolton/U72mDiJS/</t>
         </is>
       </c>
     </row>
@@ -10509,22 +10509,22 @@
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>Port Vale</t>
+          <t>Lincoln</t>
         </is>
       </c>
       <c r="G110" t="n">
+        <v>2</v>
+      </c>
+      <c r="H110" t="inlineStr">
+        <is>
+          <t>Cheltenham</t>
+        </is>
+      </c>
+      <c r="I110" t="n">
         <v>0</v>
       </c>
-      <c r="H110" t="inlineStr">
-        <is>
-          <t>Bolton</t>
-        </is>
-      </c>
-      <c r="I110" t="n">
-        <v>1</v>
-      </c>
       <c r="J110" t="n">
-        <v>3.09</v>
+        <v>1.81</v>
       </c>
       <c r="K110" t="inlineStr">
         <is>
@@ -10532,48 +10532,48 @@
         </is>
       </c>
       <c r="L110" t="n">
-        <v>2.64</v>
+        <v>1.76</v>
       </c>
       <c r="M110" t="inlineStr">
         <is>
+          <t>30/09/2023 15:39</t>
+        </is>
+      </c>
+      <c r="N110" t="n">
+        <v>3.55</v>
+      </c>
+      <c r="O110" t="inlineStr">
+        <is>
+          <t>23/09/2023 17:13</t>
+        </is>
+      </c>
+      <c r="P110" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="Q110" t="inlineStr">
+        <is>
           <t>30/09/2023 15:48</t>
         </is>
       </c>
-      <c r="N110" t="n">
-        <v>3.23</v>
-      </c>
-      <c r="O110" t="inlineStr">
+      <c r="R110" t="n">
+        <v>4.74</v>
+      </c>
+      <c r="S110" t="inlineStr">
         <is>
           <t>23/09/2023 17:13</t>
         </is>
       </c>
-      <c r="P110" t="n">
-        <v>3.49</v>
-      </c>
-      <c r="Q110" t="inlineStr">
-        <is>
-          <t>30/09/2023 15:48</t>
-        </is>
-      </c>
-      <c r="R110" t="n">
-        <v>2.44</v>
-      </c>
-      <c r="S110" t="inlineStr">
-        <is>
-          <t>23/09/2023 17:13</t>
-        </is>
-      </c>
       <c r="T110" t="n">
-        <v>2.72</v>
+        <v>5.02</v>
       </c>
       <c r="U110" t="inlineStr">
         <is>
-          <t>30/09/2023 15:48</t>
+          <t>30/09/2023 15:40</t>
         </is>
       </c>
       <c r="V110" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/port-vale-bolton/U72mDiJS/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/lincoln-city-cheltenham/Yu9vFDlG/</t>
         </is>
       </c>
     </row>
@@ -10601,71 +10601,71 @@
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>Shrewsbury</t>
+          <t>Fleetwood</t>
         </is>
       </c>
       <c r="G111" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H111" t="inlineStr">
         <is>
-          <t>Charlton</t>
+          <t>Leyton Orient</t>
         </is>
       </c>
       <c r="I111" t="n">
         <v>0</v>
       </c>
       <c r="J111" t="n">
-        <v>2.67</v>
+        <v>2.16</v>
       </c>
       <c r="K111" t="inlineStr">
         <is>
-          <t>23/09/2023 17:13</t>
+          <t>24/09/2023 03:13</t>
         </is>
       </c>
       <c r="L111" t="n">
-        <v>3.08</v>
+        <v>2.23</v>
       </c>
       <c r="M111" t="inlineStr">
         <is>
-          <t>30/09/2023 15:57</t>
+          <t>30/09/2023 15:50</t>
         </is>
       </c>
       <c r="N111" t="n">
-        <v>3.15</v>
+        <v>3.36</v>
       </c>
       <c r="O111" t="inlineStr">
         <is>
-          <t>23/09/2023 17:13</t>
+          <t>24/09/2023 03:13</t>
         </is>
       </c>
       <c r="P111" t="n">
-        <v>3.43</v>
+        <v>3.48</v>
       </c>
       <c r="Q111" t="inlineStr">
         <is>
-          <t>30/09/2023 15:18</t>
+          <t>30/09/2023 15:50</t>
         </is>
       </c>
       <c r="R111" t="n">
-        <v>2.71</v>
+        <v>3.34</v>
       </c>
       <c r="S111" t="inlineStr">
         <is>
-          <t>23/09/2023 17:13</t>
+          <t>24/09/2023 03:13</t>
         </is>
       </c>
       <c r="T111" t="n">
-        <v>2.4</v>
+        <v>3.36</v>
       </c>
       <c r="U111" t="inlineStr">
         <is>
-          <t>30/09/2023 15:57</t>
+          <t>30/09/2023 15:50</t>
         </is>
       </c>
       <c r="V111" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/shrewsbury-charlton/vslJ7Vtj/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/fleetwood-town-leyton-orient/vJ9zGgZ9/</t>
         </is>
       </c>
     </row>
@@ -10693,22 +10693,22 @@
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>Stevenage</t>
+          <t>Exeter</t>
         </is>
       </c>
       <c r="G112" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H112" t="inlineStr">
         <is>
-          <t>Oxford Utd</t>
+          <t>Northampton</t>
         </is>
       </c>
       <c r="I112" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J112" t="n">
-        <v>2.53</v>
+        <v>1.73</v>
       </c>
       <c r="K112" t="inlineStr">
         <is>
@@ -10716,7 +10716,7 @@
         </is>
       </c>
       <c r="L112" t="n">
-        <v>2.42</v>
+        <v>2.13</v>
       </c>
       <c r="M112" t="inlineStr">
         <is>
@@ -10724,7 +10724,7 @@
         </is>
       </c>
       <c r="N112" t="n">
-        <v>3.2</v>
+        <v>3.48</v>
       </c>
       <c r="O112" t="inlineStr">
         <is>
@@ -10732,7 +10732,7 @@
         </is>
       </c>
       <c r="P112" t="n">
-        <v>3.42</v>
+        <v>3.53</v>
       </c>
       <c r="Q112" t="inlineStr">
         <is>
@@ -10740,7 +10740,7 @@
         </is>
       </c>
       <c r="R112" t="n">
-        <v>2.83</v>
+        <v>5.01</v>
       </c>
       <c r="S112" t="inlineStr">
         <is>
@@ -10748,7 +10748,7 @@
         </is>
       </c>
       <c r="T112" t="n">
-        <v>3.06</v>
+        <v>3.57</v>
       </c>
       <c r="U112" t="inlineStr">
         <is>
@@ -10757,7 +10757,7 @@
       </c>
       <c r="V112" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/stevenage-oxford-utd/IXnN6kdd/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/exeter-northampton/0SAWGZJ3/</t>
         </is>
       </c>
     </row>
@@ -10785,71 +10785,71 @@
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>Wigan</t>
+          <t>Derby</t>
         </is>
       </c>
       <c r="G113" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H113" t="inlineStr">
         <is>
-          <t>Portsmouth</t>
+          <t>Cambridge Utd</t>
         </is>
       </c>
       <c r="I113" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J113" t="n">
-        <v>3.14</v>
+        <v>1.56</v>
       </c>
       <c r="K113" t="inlineStr">
         <is>
-          <t>24/09/2023 03:13</t>
+          <t>23/09/2023 17:13</t>
         </is>
       </c>
       <c r="L113" t="n">
-        <v>3.11</v>
+        <v>1.64</v>
       </c>
       <c r="M113" t="inlineStr">
         <is>
-          <t>30/09/2023 14:21</t>
+          <t>30/09/2023 15:58</t>
         </is>
       </c>
       <c r="N113" t="n">
-        <v>3.21</v>
+        <v>4.18</v>
       </c>
       <c r="O113" t="inlineStr">
         <is>
-          <t>24/09/2023 03:13</t>
+          <t>23/09/2023 17:13</t>
         </is>
       </c>
       <c r="P113" t="n">
-        <v>3.59</v>
+        <v>4.2</v>
       </c>
       <c r="Q113" t="inlineStr">
         <is>
-          <t>30/09/2023 15:38</t>
+          <t>30/09/2023 15:58</t>
         </is>
       </c>
       <c r="R113" t="n">
-        <v>2.42</v>
+        <v>5.3</v>
       </c>
       <c r="S113" t="inlineStr">
         <is>
-          <t>24/09/2023 03:13</t>
+          <t>23/09/2023 17:13</t>
         </is>
       </c>
       <c r="T113" t="n">
-        <v>2.31</v>
+        <v>5.29</v>
       </c>
       <c r="U113" t="inlineStr">
         <is>
-          <t>30/09/2023 14:21</t>
+          <t>30/09/2023 15:58</t>
         </is>
       </c>
       <c r="V113" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/wigan-portsmouth/KxR5VYYd/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/derby-cambridge-utd/riGRHF4c/</t>
         </is>
       </c>
     </row>
@@ -10877,22 +10877,22 @@
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>Wycombe</t>
+          <t>Barnsley</t>
         </is>
       </c>
       <c r="G114" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H114" t="inlineStr">
         <is>
-          <t>Carlisle</t>
+          <t>Blackpool</t>
         </is>
       </c>
       <c r="I114" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J114" t="n">
-        <v>1.78</v>
+        <v>2.18</v>
       </c>
       <c r="K114" t="inlineStr">
         <is>
@@ -10900,48 +10900,48 @@
         </is>
       </c>
       <c r="L114" t="n">
-        <v>1.96</v>
+        <v>2.51</v>
       </c>
       <c r="M114" t="inlineStr">
         <is>
+          <t>30/09/2023 15:50</t>
+        </is>
+      </c>
+      <c r="N114" t="n">
+        <v>3.31</v>
+      </c>
+      <c r="O114" t="inlineStr">
+        <is>
+          <t>24/09/2023 03:13</t>
+        </is>
+      </c>
+      <c r="P114" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="Q114" t="inlineStr">
+        <is>
+          <t>30/09/2023 15:50</t>
+        </is>
+      </c>
+      <c r="R114" t="n">
+        <v>3.55</v>
+      </c>
+      <c r="S114" t="inlineStr">
+        <is>
+          <t>24/09/2023 03:13</t>
+        </is>
+      </c>
+      <c r="T114" t="n">
+        <v>2.81</v>
+      </c>
+      <c r="U114" t="inlineStr">
+        <is>
           <t>30/09/2023 15:51</t>
         </is>
       </c>
-      <c r="N114" t="n">
-        <v>3.7</v>
-      </c>
-      <c r="O114" t="inlineStr">
-        <is>
-          <t>24/09/2023 03:13</t>
-        </is>
-      </c>
-      <c r="P114" t="n">
-        <v>3.41</v>
-      </c>
-      <c r="Q114" t="inlineStr">
-        <is>
-          <t>30/09/2023 15:51</t>
-        </is>
-      </c>
-      <c r="R114" t="n">
-        <v>4.31</v>
-      </c>
-      <c r="S114" t="inlineStr">
-        <is>
-          <t>24/09/2023 03:13</t>
-        </is>
-      </c>
-      <c r="T114" t="n">
-        <v>4.31</v>
-      </c>
-      <c r="U114" t="inlineStr">
-        <is>
-          <t>30/09/2023 15:51</t>
-        </is>
-      </c>
       <c r="V114" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/wycombe-carlisle/YuV9Uhl3/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/barnsley-blackpool/40HNIeki/</t>
         </is>
       </c>
     </row>
@@ -10969,22 +10969,22 @@
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>Cheltenham</t>
+          <t>Portsmouth</t>
         </is>
       </c>
       <c r="G115" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H115" t="inlineStr">
         <is>
-          <t>Fleetwood</t>
+          <t>Wycombe</t>
         </is>
       </c>
       <c r="I115" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J115" t="n">
-        <v>2.98</v>
+        <v>1.78</v>
       </c>
       <c r="K115" t="inlineStr">
         <is>
@@ -10992,15 +10992,15 @@
         </is>
       </c>
       <c r="L115" t="n">
-        <v>3.37</v>
+        <v>1.8</v>
       </c>
       <c r="M115" t="inlineStr">
         <is>
-          <t>03/10/2023 20:30</t>
+          <t>03/10/2023 19:21</t>
         </is>
       </c>
       <c r="N115" t="n">
-        <v>3.32</v>
+        <v>3.78</v>
       </c>
       <c r="O115" t="inlineStr">
         <is>
@@ -11008,15 +11008,15 @@
         </is>
       </c>
       <c r="P115" t="n">
-        <v>3.19</v>
+        <v>3.72</v>
       </c>
       <c r="Q115" t="inlineStr">
         <is>
-          <t>03/10/2023 20:08</t>
+          <t>03/10/2023 19:57</t>
         </is>
       </c>
       <c r="R115" t="n">
-        <v>2.36</v>
+        <v>4.57</v>
       </c>
       <c r="S115" t="inlineStr">
         <is>
@@ -11024,16 +11024,16 @@
         </is>
       </c>
       <c r="T115" t="n">
-        <v>2.36</v>
+        <v>4.73</v>
       </c>
       <c r="U115" t="inlineStr">
         <is>
-          <t>03/10/2023 20:30</t>
+          <t>03/10/2023 19:57</t>
         </is>
       </c>
       <c r="V115" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/cheltenham-fleetwood-town/hj15JSu2/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/portsmouth-wycombe/GOn0uA2L/</t>
         </is>
       </c>
     </row>
@@ -11061,7 +11061,7 @@
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>Northampton</t>
+          <t>Oxford Utd</t>
         </is>
       </c>
       <c r="G116" t="n">
@@ -11069,63 +11069,63 @@
       </c>
       <c r="H116" t="inlineStr">
         <is>
-          <t>Reading</t>
+          <t>Shrewsbury</t>
         </is>
       </c>
       <c r="I116" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J116" t="n">
-        <v>2.41</v>
+        <v>1.56</v>
       </c>
       <c r="K116" t="inlineStr">
         <is>
-          <t>30/09/2023 22:42</t>
+          <t>30/09/2023 17:13</t>
         </is>
       </c>
       <c r="L116" t="n">
-        <v>2.43</v>
+        <v>1.53</v>
       </c>
       <c r="M116" t="inlineStr">
         <is>
-          <t>03/10/2023 20:44</t>
+          <t>03/10/2023 20:33</t>
         </is>
       </c>
       <c r="N116" t="n">
-        <v>3.49</v>
+        <v>4.11</v>
       </c>
       <c r="O116" t="inlineStr">
         <is>
-          <t>30/09/2023 22:42</t>
+          <t>30/09/2023 17:13</t>
         </is>
       </c>
       <c r="P116" t="n">
-        <v>3.54</v>
+        <v>4.21</v>
       </c>
       <c r="Q116" t="inlineStr">
         <is>
-          <t>03/10/2023 20:44</t>
+          <t>03/10/2023 20:33</t>
         </is>
       </c>
       <c r="R116" t="n">
-        <v>2.79</v>
+        <v>6.08</v>
       </c>
       <c r="S116" t="inlineStr">
         <is>
-          <t>30/09/2023 22:42</t>
+          <t>30/09/2023 17:13</t>
         </is>
       </c>
       <c r="T116" t="n">
-        <v>2.95</v>
+        <v>6.92</v>
       </c>
       <c r="U116" t="inlineStr">
         <is>
-          <t>03/10/2023 20:44</t>
+          <t>03/10/2023 20:33</t>
         </is>
       </c>
       <c r="V116" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/northampton-reading/KdgisWX8/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/oxford-utd-shrewsbury/2LrdtjmF/</t>
         </is>
       </c>
     </row>
@@ -11153,71 +11153,71 @@
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>Cambridge Utd</t>
+          <t>Northampton</t>
         </is>
       </c>
       <c r="G117" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H117" t="inlineStr">
         <is>
-          <t>Barnsley</t>
+          <t>Reading</t>
         </is>
       </c>
       <c r="I117" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J117" t="n">
-        <v>2.61</v>
+        <v>2.41</v>
       </c>
       <c r="K117" t="inlineStr">
         <is>
-          <t>30/09/2023 17:13</t>
+          <t>30/09/2023 22:42</t>
         </is>
       </c>
       <c r="L117" t="n">
-        <v>2.84</v>
+        <v>2.43</v>
       </c>
       <c r="M117" t="inlineStr">
         <is>
-          <t>03/10/2023 20:19</t>
+          <t>03/10/2023 20:44</t>
         </is>
       </c>
       <c r="N117" t="n">
-        <v>3.37</v>
+        <v>3.49</v>
       </c>
       <c r="O117" t="inlineStr">
         <is>
-          <t>30/09/2023 17:13</t>
+          <t>30/09/2023 22:42</t>
         </is>
       </c>
       <c r="P117" t="n">
-        <v>3.52</v>
+        <v>3.54</v>
       </c>
       <c r="Q117" t="inlineStr">
         <is>
-          <t>03/10/2023 20:19</t>
+          <t>03/10/2023 20:44</t>
         </is>
       </c>
       <c r="R117" t="n">
-        <v>2.64</v>
+        <v>2.79</v>
       </c>
       <c r="S117" t="inlineStr">
         <is>
-          <t>30/09/2023 17:13</t>
+          <t>30/09/2023 22:42</t>
         </is>
       </c>
       <c r="T117" t="n">
-        <v>2.52</v>
+        <v>2.95</v>
       </c>
       <c r="U117" t="inlineStr">
         <is>
-          <t>03/10/2023 20:19</t>
+          <t>03/10/2023 20:44</t>
         </is>
       </c>
       <c r="V117" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/cambridge-utd-barnsley/K09hMUeq/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/northampton-reading/KdgisWX8/</t>
         </is>
       </c>
     </row>
@@ -11245,22 +11245,22 @@
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>Portsmouth</t>
+          <t>Cheltenham</t>
         </is>
       </c>
       <c r="G118" t="n">
+        <v>0</v>
+      </c>
+      <c r="H118" t="inlineStr">
+        <is>
+          <t>Fleetwood</t>
+        </is>
+      </c>
+      <c r="I118" t="n">
         <v>2</v>
       </c>
-      <c r="H118" t="inlineStr">
-        <is>
-          <t>Wycombe</t>
-        </is>
-      </c>
-      <c r="I118" t="n">
-        <v>1</v>
-      </c>
       <c r="J118" t="n">
-        <v>1.78</v>
+        <v>2.98</v>
       </c>
       <c r="K118" t="inlineStr">
         <is>
@@ -11268,15 +11268,15 @@
         </is>
       </c>
       <c r="L118" t="n">
-        <v>1.8</v>
+        <v>3.37</v>
       </c>
       <c r="M118" t="inlineStr">
         <is>
-          <t>03/10/2023 19:21</t>
+          <t>03/10/2023 20:30</t>
         </is>
       </c>
       <c r="N118" t="n">
-        <v>3.78</v>
+        <v>3.32</v>
       </c>
       <c r="O118" t="inlineStr">
         <is>
@@ -11284,15 +11284,15 @@
         </is>
       </c>
       <c r="P118" t="n">
-        <v>3.72</v>
+        <v>3.19</v>
       </c>
       <c r="Q118" t="inlineStr">
         <is>
-          <t>03/10/2023 19:57</t>
+          <t>03/10/2023 20:08</t>
         </is>
       </c>
       <c r="R118" t="n">
-        <v>4.57</v>
+        <v>2.36</v>
       </c>
       <c r="S118" t="inlineStr">
         <is>
@@ -11300,16 +11300,16 @@
         </is>
       </c>
       <c r="T118" t="n">
-        <v>4.73</v>
+        <v>2.36</v>
       </c>
       <c r="U118" t="inlineStr">
         <is>
-          <t>03/10/2023 19:57</t>
+          <t>03/10/2023 20:30</t>
         </is>
       </c>
       <c r="V118" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/portsmouth-wycombe/GOn0uA2L/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/cheltenham-fleetwood-town/hj15JSu2/</t>
         </is>
       </c>
     </row>
@@ -11337,22 +11337,22 @@
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>Oxford Utd</t>
+          <t>Charlton</t>
         </is>
       </c>
       <c r="G119" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H119" t="inlineStr">
         <is>
-          <t>Shrewsbury</t>
+          <t>Exeter</t>
         </is>
       </c>
       <c r="I119" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J119" t="n">
-        <v>1.56</v>
+        <v>2.17</v>
       </c>
       <c r="K119" t="inlineStr">
         <is>
@@ -11360,15 +11360,15 @@
         </is>
       </c>
       <c r="L119" t="n">
-        <v>1.53</v>
+        <v>1.87</v>
       </c>
       <c r="M119" t="inlineStr">
         <is>
-          <t>03/10/2023 20:33</t>
+          <t>03/10/2023 20:35</t>
         </is>
       </c>
       <c r="N119" t="n">
-        <v>4.11</v>
+        <v>3.49</v>
       </c>
       <c r="O119" t="inlineStr">
         <is>
@@ -11376,15 +11376,15 @@
         </is>
       </c>
       <c r="P119" t="n">
-        <v>4.21</v>
+        <v>3.83</v>
       </c>
       <c r="Q119" t="inlineStr">
         <is>
-          <t>03/10/2023 20:33</t>
+          <t>03/10/2023 20:35</t>
         </is>
       </c>
       <c r="R119" t="n">
-        <v>6.08</v>
+        <v>3.38</v>
       </c>
       <c r="S119" t="inlineStr">
         <is>
@@ -11392,16 +11392,16 @@
         </is>
       </c>
       <c r="T119" t="n">
-        <v>6.92</v>
+        <v>4.17</v>
       </c>
       <c r="U119" t="inlineStr">
         <is>
-          <t>03/10/2023 20:33</t>
+          <t>03/10/2023 20:35</t>
         </is>
       </c>
       <c r="V119" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/oxford-utd-shrewsbury/2LrdtjmF/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/charlton-exeter/Ea21K8Qe/</t>
         </is>
       </c>
     </row>
@@ -11429,71 +11429,71 @@
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>Charlton</t>
+          <t>Burton</t>
         </is>
       </c>
       <c r="G120" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H120" t="inlineStr">
         <is>
-          <t>Exeter</t>
+          <t>Wigan</t>
         </is>
       </c>
       <c r="I120" t="n">
         <v>1</v>
       </c>
       <c r="J120" t="n">
-        <v>2.17</v>
+        <v>2.98</v>
       </c>
       <c r="K120" t="inlineStr">
         <is>
-          <t>30/09/2023 17:13</t>
+          <t>30/09/2023 22:42</t>
         </is>
       </c>
       <c r="L120" t="n">
-        <v>1.87</v>
+        <v>2.62</v>
       </c>
       <c r="M120" t="inlineStr">
         <is>
-          <t>03/10/2023 20:35</t>
+          <t>03/10/2023 20:31</t>
         </is>
       </c>
       <c r="N120" t="n">
-        <v>3.49</v>
+        <v>3.44</v>
       </c>
       <c r="O120" t="inlineStr">
         <is>
-          <t>30/09/2023 17:13</t>
+          <t>30/09/2023 22:42</t>
         </is>
       </c>
       <c r="P120" t="n">
-        <v>3.83</v>
+        <v>3.28</v>
       </c>
       <c r="Q120" t="inlineStr">
         <is>
-          <t>03/10/2023 20:35</t>
+          <t>03/10/2023 20:22</t>
         </is>
       </c>
       <c r="R120" t="n">
-        <v>3.38</v>
+        <v>2.4</v>
       </c>
       <c r="S120" t="inlineStr">
         <is>
-          <t>30/09/2023 17:13</t>
+          <t>30/09/2023 22:42</t>
         </is>
       </c>
       <c r="T120" t="n">
-        <v>4.17</v>
+        <v>2.88</v>
       </c>
       <c r="U120" t="inlineStr">
         <is>
-          <t>03/10/2023 20:35</t>
+          <t>03/10/2023 20:31</t>
         </is>
       </c>
       <c r="V120" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/charlton-exeter/Ea21K8Qe/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/burton-wigan/2LMQQAmS/</t>
         </is>
       </c>
     </row>
@@ -11521,71 +11521,71 @@
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>Burton</t>
+          <t>Cambridge Utd</t>
         </is>
       </c>
       <c r="G121" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H121" t="inlineStr">
         <is>
-          <t>Wigan</t>
+          <t>Barnsley</t>
         </is>
       </c>
       <c r="I121" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J121" t="n">
-        <v>2.98</v>
+        <v>2.61</v>
       </c>
       <c r="K121" t="inlineStr">
         <is>
-          <t>30/09/2023 22:42</t>
+          <t>30/09/2023 17:13</t>
         </is>
       </c>
       <c r="L121" t="n">
-        <v>2.62</v>
+        <v>2.84</v>
       </c>
       <c r="M121" t="inlineStr">
         <is>
-          <t>03/10/2023 20:31</t>
+          <t>03/10/2023 20:19</t>
         </is>
       </c>
       <c r="N121" t="n">
-        <v>3.44</v>
+        <v>3.37</v>
       </c>
       <c r="O121" t="inlineStr">
         <is>
-          <t>30/09/2023 22:42</t>
+          <t>30/09/2023 17:13</t>
         </is>
       </c>
       <c r="P121" t="n">
-        <v>3.28</v>
+        <v>3.52</v>
       </c>
       <c r="Q121" t="inlineStr">
         <is>
-          <t>03/10/2023 20:22</t>
+          <t>03/10/2023 20:19</t>
         </is>
       </c>
       <c r="R121" t="n">
-        <v>2.4</v>
+        <v>2.64</v>
       </c>
       <c r="S121" t="inlineStr">
         <is>
-          <t>30/09/2023 22:42</t>
+          <t>30/09/2023 17:13</t>
         </is>
       </c>
       <c r="T121" t="n">
-        <v>2.88</v>
+        <v>2.52</v>
       </c>
       <c r="U121" t="inlineStr">
         <is>
-          <t>03/10/2023 20:31</t>
+          <t>03/10/2023 20:19</t>
         </is>
       </c>
       <c r="V121" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/burton-wigan/2LMQQAmS/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/cambridge-utd-barnsley/K09hMUeq/</t>
         </is>
       </c>
     </row>
@@ -12073,22 +12073,22 @@
       </c>
       <c r="F127" t="inlineStr">
         <is>
-          <t>Exeter</t>
+          <t>Stevenage</t>
         </is>
       </c>
       <c r="G127" t="n">
+        <v>1</v>
+      </c>
+      <c r="H127" t="inlineStr">
+        <is>
+          <t>Wigan</t>
+        </is>
+      </c>
+      <c r="I127" t="n">
         <v>0</v>
       </c>
-      <c r="H127" t="inlineStr">
-        <is>
-          <t>Barnsley</t>
-        </is>
-      </c>
-      <c r="I127" t="n">
-        <v>1</v>
-      </c>
       <c r="J127" t="n">
-        <v>2.26</v>
+        <v>1.78</v>
       </c>
       <c r="K127" t="inlineStr">
         <is>
@@ -12096,15 +12096,15 @@
         </is>
       </c>
       <c r="L127" t="n">
-        <v>2.93</v>
+        <v>1.82</v>
       </c>
       <c r="M127" t="inlineStr">
         <is>
-          <t>07/10/2023 15:52</t>
+          <t>07/10/2023 15:49</t>
         </is>
       </c>
       <c r="N127" t="n">
-        <v>3.38</v>
+        <v>3.81</v>
       </c>
       <c r="O127" t="inlineStr">
         <is>
@@ -12112,15 +12112,15 @@
         </is>
       </c>
       <c r="P127" t="n">
-        <v>3.46</v>
+        <v>3.61</v>
       </c>
       <c r="Q127" t="inlineStr">
         <is>
-          <t>07/10/2023 15:52</t>
+          <t>07/10/2023 15:49</t>
         </is>
       </c>
       <c r="R127" t="n">
-        <v>3.11</v>
+        <v>4.15</v>
       </c>
       <c r="S127" t="inlineStr">
         <is>
@@ -12128,16 +12128,16 @@
         </is>
       </c>
       <c r="T127" t="n">
-        <v>2.48</v>
+        <v>4.8</v>
       </c>
       <c r="U127" t="inlineStr">
         <is>
-          <t>07/10/2023 15:52</t>
+          <t>07/10/2023 15:49</t>
         </is>
       </c>
       <c r="V127" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/exeter-barnsley/CU2zXoA1/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/stevenage-wigan/6R47ZvWa/</t>
         </is>
       </c>
     </row>
@@ -12165,7 +12165,7 @@
       </c>
       <c r="F128" t="inlineStr">
         <is>
-          <t>Bolton</t>
+          <t>Shrewsbury</t>
         </is>
       </c>
       <c r="G128" t="n">
@@ -12173,14 +12173,14 @@
       </c>
       <c r="H128" t="inlineStr">
         <is>
-          <t>Carlisle</t>
+          <t>Northampton</t>
         </is>
       </c>
       <c r="I128" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J128" t="n">
-        <v>1.6</v>
+        <v>2.41</v>
       </c>
       <c r="K128" t="inlineStr">
         <is>
@@ -12188,15 +12188,15 @@
         </is>
       </c>
       <c r="L128" t="n">
-        <v>1.55</v>
+        <v>3.03</v>
       </c>
       <c r="M128" t="inlineStr">
         <is>
-          <t>07/10/2023 16:00</t>
+          <t>07/10/2023 15:58</t>
         </is>
       </c>
       <c r="N128" t="n">
-        <v>4.06</v>
+        <v>3.33</v>
       </c>
       <c r="O128" t="inlineStr">
         <is>
@@ -12204,15 +12204,15 @@
         </is>
       </c>
       <c r="P128" t="n">
-        <v>4.29</v>
+        <v>3.19</v>
       </c>
       <c r="Q128" t="inlineStr">
         <is>
-          <t>07/10/2023 16:00</t>
+          <t>07/10/2023 15:58</t>
         </is>
       </c>
       <c r="R128" t="n">
-        <v>5.69</v>
+        <v>2.9</v>
       </c>
       <c r="S128" t="inlineStr">
         <is>
@@ -12220,16 +12220,16 @@
         </is>
       </c>
       <c r="T128" t="n">
-        <v>6.25</v>
+        <v>2.57</v>
       </c>
       <c r="U128" t="inlineStr">
         <is>
-          <t>07/10/2023 16:00</t>
+          <t>07/10/2023 15:58</t>
         </is>
       </c>
       <c r="V128" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/bolton-carlisle/Aon4vUHR/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/shrewsbury-northampton/fi13zLGg/</t>
         </is>
       </c>
     </row>
@@ -12257,7 +12257,7 @@
       </c>
       <c r="F129" t="inlineStr">
         <is>
-          <t>Charlton</t>
+          <t>Portsmouth</t>
         </is>
       </c>
       <c r="G129" t="n">
@@ -12265,14 +12265,14 @@
       </c>
       <c r="H129" t="inlineStr">
         <is>
-          <t>Blackpool</t>
+          <t>Port Vale</t>
         </is>
       </c>
       <c r="I129" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J129" t="n">
-        <v>2.5</v>
+        <v>1.66</v>
       </c>
       <c r="K129" t="inlineStr">
         <is>
@@ -12280,15 +12280,15 @@
         </is>
       </c>
       <c r="L129" t="n">
-        <v>2.36</v>
+        <v>1.6</v>
       </c>
       <c r="M129" t="inlineStr">
         <is>
-          <t>07/10/2023 15:53</t>
+          <t>07/10/2023 15:57</t>
         </is>
       </c>
       <c r="N129" t="n">
-        <v>3.32</v>
+        <v>3.95</v>
       </c>
       <c r="O129" t="inlineStr">
         <is>
@@ -12296,15 +12296,15 @@
         </is>
       </c>
       <c r="P129" t="n">
-        <v>3.41</v>
+        <v>4.37</v>
       </c>
       <c r="Q129" t="inlineStr">
         <is>
-          <t>07/10/2023 15:51</t>
+          <t>07/10/2023 15:57</t>
         </is>
       </c>
       <c r="R129" t="n">
-        <v>2.79</v>
+        <v>5.22</v>
       </c>
       <c r="S129" t="inlineStr">
         <is>
@@ -12312,16 +12312,16 @@
         </is>
       </c>
       <c r="T129" t="n">
-        <v>3.15</v>
+        <v>5.52</v>
       </c>
       <c r="U129" t="inlineStr">
         <is>
-          <t>07/10/2023 15:53</t>
+          <t>07/10/2023 15:57</t>
         </is>
       </c>
       <c r="V129" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/charlton-blackpool/vH4SY7uk/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/portsmouth-port-vale/CSBby11m/</t>
         </is>
       </c>
     </row>
@@ -12349,22 +12349,22 @@
       </c>
       <c r="F130" t="inlineStr">
         <is>
-          <t>Cheltenham</t>
+          <t>Peterborough</t>
         </is>
       </c>
       <c r="G130" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H130" t="inlineStr">
         <is>
-          <t>Derby</t>
+          <t>Lincoln</t>
         </is>
       </c>
       <c r="I130" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J130" t="n">
-        <v>4.29</v>
+        <v>1.76</v>
       </c>
       <c r="K130" t="inlineStr">
         <is>
@@ -12372,15 +12372,15 @@
         </is>
       </c>
       <c r="L130" t="n">
-        <v>6.41</v>
+        <v>1.61</v>
       </c>
       <c r="M130" t="inlineStr">
         <is>
-          <t>07/10/2023 15:39</t>
+          <t>07/10/2023 15:52</t>
         </is>
       </c>
       <c r="N130" t="n">
-        <v>3.7</v>
+        <v>3.75</v>
       </c>
       <c r="O130" t="inlineStr">
         <is>
@@ -12388,15 +12388,15 @@
         </is>
       </c>
       <c r="P130" t="n">
-        <v>4.02</v>
+        <v>4.07</v>
       </c>
       <c r="Q130" t="inlineStr">
         <is>
-          <t>07/10/2023 15:39</t>
+          <t>07/10/2023 16:00</t>
         </is>
       </c>
       <c r="R130" t="n">
-        <v>1.78</v>
+        <v>4.71</v>
       </c>
       <c r="S130" t="inlineStr">
         <is>
@@ -12404,16 +12404,16 @@
         </is>
       </c>
       <c r="T130" t="n">
-        <v>1.58</v>
+        <v>5.88</v>
       </c>
       <c r="U130" t="inlineStr">
         <is>
-          <t>07/10/2023 15:39</t>
+          <t>07/10/2023 16:00</t>
         </is>
       </c>
       <c r="V130" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/cheltenham-derby/I73WXRfe/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/peterborough-lincoln-city/YyDfxsns/</t>
         </is>
       </c>
     </row>
@@ -12441,22 +12441,22 @@
       </c>
       <c r="F131" t="inlineStr">
         <is>
-          <t>Fleetwood</t>
+          <t>Leyton Orient</t>
         </is>
       </c>
       <c r="G131" t="n">
+        <v>2</v>
+      </c>
+      <c r="H131" t="inlineStr">
+        <is>
+          <t>Reading</t>
+        </is>
+      </c>
+      <c r="I131" t="n">
         <v>1</v>
       </c>
-      <c r="H131" t="inlineStr">
-        <is>
-          <t>Wycombe</t>
-        </is>
-      </c>
-      <c r="I131" t="n">
-        <v>4</v>
-      </c>
       <c r="J131" t="n">
-        <v>2.43</v>
+        <v>2.14</v>
       </c>
       <c r="K131" t="inlineStr">
         <is>
@@ -12464,15 +12464,15 @@
         </is>
       </c>
       <c r="L131" t="n">
-        <v>2.29</v>
+        <v>2.4</v>
       </c>
       <c r="M131" t="inlineStr">
         <is>
-          <t>07/10/2023 15:50</t>
+          <t>07/10/2023 15:57</t>
         </is>
       </c>
       <c r="N131" t="n">
-        <v>3.27</v>
+        <v>3.35</v>
       </c>
       <c r="O131" t="inlineStr">
         <is>
@@ -12480,15 +12480,15 @@
         </is>
       </c>
       <c r="P131" t="n">
-        <v>3.37</v>
+        <v>3.35</v>
       </c>
       <c r="Q131" t="inlineStr">
         <is>
-          <t>07/10/2023 15:46</t>
+          <t>07/10/2023 15:52</t>
         </is>
       </c>
       <c r="R131" t="n">
-        <v>3.07</v>
+        <v>3.39</v>
       </c>
       <c r="S131" t="inlineStr">
         <is>
@@ -12496,16 +12496,16 @@
         </is>
       </c>
       <c r="T131" t="n">
-        <v>3.34</v>
+        <v>3.14</v>
       </c>
       <c r="U131" t="inlineStr">
         <is>
-          <t>07/10/2023 15:50</t>
+          <t>07/10/2023 15:52</t>
         </is>
       </c>
       <c r="V131" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/fleetwood-town-wycombe/QX6vW5P7/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/leyton-orient-reading/SxoNfk28/</t>
         </is>
       </c>
     </row>
@@ -12533,22 +12533,22 @@
       </c>
       <c r="F132" t="inlineStr">
         <is>
-          <t>Leyton Orient</t>
+          <t>Cheltenham</t>
         </is>
       </c>
       <c r="G132" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H132" t="inlineStr">
         <is>
-          <t>Reading</t>
+          <t>Derby</t>
         </is>
       </c>
       <c r="I132" t="n">
         <v>1</v>
       </c>
       <c r="J132" t="n">
-        <v>2.14</v>
+        <v>4.29</v>
       </c>
       <c r="K132" t="inlineStr">
         <is>
@@ -12556,15 +12556,15 @@
         </is>
       </c>
       <c r="L132" t="n">
-        <v>2.4</v>
+        <v>6.41</v>
       </c>
       <c r="M132" t="inlineStr">
         <is>
-          <t>07/10/2023 15:57</t>
+          <t>07/10/2023 15:39</t>
         </is>
       </c>
       <c r="N132" t="n">
-        <v>3.35</v>
+        <v>3.7</v>
       </c>
       <c r="O132" t="inlineStr">
         <is>
@@ -12572,15 +12572,15 @@
         </is>
       </c>
       <c r="P132" t="n">
-        <v>3.35</v>
+        <v>4.02</v>
       </c>
       <c r="Q132" t="inlineStr">
         <is>
-          <t>07/10/2023 15:52</t>
+          <t>07/10/2023 15:39</t>
         </is>
       </c>
       <c r="R132" t="n">
-        <v>3.39</v>
+        <v>1.78</v>
       </c>
       <c r="S132" t="inlineStr">
         <is>
@@ -12588,16 +12588,16 @@
         </is>
       </c>
       <c r="T132" t="n">
-        <v>3.14</v>
+        <v>1.58</v>
       </c>
       <c r="U132" t="inlineStr">
         <is>
-          <t>07/10/2023 15:52</t>
+          <t>07/10/2023 15:39</t>
         </is>
       </c>
       <c r="V132" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/leyton-orient-reading/SxoNfk28/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/cheltenham-derby/I73WXRfe/</t>
         </is>
       </c>
     </row>
@@ -12625,22 +12625,22 @@
       </c>
       <c r="F133" t="inlineStr">
         <is>
-          <t>Peterborough</t>
+          <t>Exeter</t>
         </is>
       </c>
       <c r="G133" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H133" t="inlineStr">
         <is>
-          <t>Lincoln</t>
+          <t>Barnsley</t>
         </is>
       </c>
       <c r="I133" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J133" t="n">
-        <v>1.76</v>
+        <v>2.26</v>
       </c>
       <c r="K133" t="inlineStr">
         <is>
@@ -12648,7 +12648,7 @@
         </is>
       </c>
       <c r="L133" t="n">
-        <v>1.61</v>
+        <v>2.93</v>
       </c>
       <c r="M133" t="inlineStr">
         <is>
@@ -12656,7 +12656,7 @@
         </is>
       </c>
       <c r="N133" t="n">
-        <v>3.75</v>
+        <v>3.38</v>
       </c>
       <c r="O133" t="inlineStr">
         <is>
@@ -12664,15 +12664,15 @@
         </is>
       </c>
       <c r="P133" t="n">
-        <v>4.07</v>
+        <v>3.46</v>
       </c>
       <c r="Q133" t="inlineStr">
         <is>
-          <t>07/10/2023 16:00</t>
+          <t>07/10/2023 15:52</t>
         </is>
       </c>
       <c r="R133" t="n">
-        <v>4.71</v>
+        <v>3.11</v>
       </c>
       <c r="S133" t="inlineStr">
         <is>
@@ -12680,16 +12680,16 @@
         </is>
       </c>
       <c r="T133" t="n">
-        <v>5.88</v>
+        <v>2.48</v>
       </c>
       <c r="U133" t="inlineStr">
         <is>
-          <t>07/10/2023 16:00</t>
+          <t>07/10/2023 15:52</t>
         </is>
       </c>
       <c r="V133" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/peterborough-lincoln-city/YyDfxsns/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/exeter-barnsley/CU2zXoA1/</t>
         </is>
       </c>
     </row>
@@ -12717,7 +12717,7 @@
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>Portsmouth</t>
+          <t>Charlton</t>
         </is>
       </c>
       <c r="G134" t="n">
@@ -12725,14 +12725,14 @@
       </c>
       <c r="H134" t="inlineStr">
         <is>
-          <t>Port Vale</t>
+          <t>Blackpool</t>
         </is>
       </c>
       <c r="I134" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J134" t="n">
-        <v>1.66</v>
+        <v>2.5</v>
       </c>
       <c r="K134" t="inlineStr">
         <is>
@@ -12740,15 +12740,15 @@
         </is>
       </c>
       <c r="L134" t="n">
-        <v>1.6</v>
+        <v>2.36</v>
       </c>
       <c r="M134" t="inlineStr">
         <is>
-          <t>07/10/2023 15:57</t>
+          <t>07/10/2023 15:53</t>
         </is>
       </c>
       <c r="N134" t="n">
-        <v>3.95</v>
+        <v>3.32</v>
       </c>
       <c r="O134" t="inlineStr">
         <is>
@@ -12756,15 +12756,15 @@
         </is>
       </c>
       <c r="P134" t="n">
-        <v>4.37</v>
+        <v>3.41</v>
       </c>
       <c r="Q134" t="inlineStr">
         <is>
-          <t>07/10/2023 15:57</t>
+          <t>07/10/2023 15:51</t>
         </is>
       </c>
       <c r="R134" t="n">
-        <v>5.22</v>
+        <v>2.79</v>
       </c>
       <c r="S134" t="inlineStr">
         <is>
@@ -12772,16 +12772,16 @@
         </is>
       </c>
       <c r="T134" t="n">
-        <v>5.52</v>
+        <v>3.15</v>
       </c>
       <c r="U134" t="inlineStr">
         <is>
-          <t>07/10/2023 15:57</t>
+          <t>07/10/2023 15:53</t>
         </is>
       </c>
       <c r="V134" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/portsmouth-port-vale/CSBby11m/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/charlton-blackpool/vH4SY7uk/</t>
         </is>
       </c>
     </row>
@@ -12809,7 +12809,7 @@
       </c>
       <c r="F135" t="inlineStr">
         <is>
-          <t>Shrewsbury</t>
+          <t>Bolton</t>
         </is>
       </c>
       <c r="G135" t="n">
@@ -12817,14 +12817,14 @@
       </c>
       <c r="H135" t="inlineStr">
         <is>
-          <t>Northampton</t>
+          <t>Carlisle</t>
         </is>
       </c>
       <c r="I135" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J135" t="n">
-        <v>2.41</v>
+        <v>1.6</v>
       </c>
       <c r="K135" t="inlineStr">
         <is>
@@ -12832,15 +12832,15 @@
         </is>
       </c>
       <c r="L135" t="n">
-        <v>3.03</v>
+        <v>1.55</v>
       </c>
       <c r="M135" t="inlineStr">
         <is>
-          <t>07/10/2023 15:58</t>
+          <t>07/10/2023 16:00</t>
         </is>
       </c>
       <c r="N135" t="n">
-        <v>3.33</v>
+        <v>4.06</v>
       </c>
       <c r="O135" t="inlineStr">
         <is>
@@ -12848,15 +12848,15 @@
         </is>
       </c>
       <c r="P135" t="n">
-        <v>3.19</v>
+        <v>4.29</v>
       </c>
       <c r="Q135" t="inlineStr">
         <is>
-          <t>07/10/2023 15:58</t>
+          <t>07/10/2023 16:00</t>
         </is>
       </c>
       <c r="R135" t="n">
-        <v>2.9</v>
+        <v>5.69</v>
       </c>
       <c r="S135" t="inlineStr">
         <is>
@@ -12864,16 +12864,16 @@
         </is>
       </c>
       <c r="T135" t="n">
-        <v>2.57</v>
+        <v>6.25</v>
       </c>
       <c r="U135" t="inlineStr">
         <is>
-          <t>07/10/2023 15:58</t>
+          <t>07/10/2023 16:00</t>
         </is>
       </c>
       <c r="V135" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/shrewsbury-northampton/fi13zLGg/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/bolton-carlisle/Aon4vUHR/</t>
         </is>
       </c>
     </row>
@@ -12901,7 +12901,7 @@
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>Stevenage</t>
+          <t>Fleetwood</t>
         </is>
       </c>
       <c r="G136" t="n">
@@ -12909,14 +12909,14 @@
       </c>
       <c r="H136" t="inlineStr">
         <is>
-          <t>Wigan</t>
+          <t>Wycombe</t>
         </is>
       </c>
       <c r="I136" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J136" t="n">
-        <v>1.78</v>
+        <v>2.43</v>
       </c>
       <c r="K136" t="inlineStr">
         <is>
@@ -12924,15 +12924,15 @@
         </is>
       </c>
       <c r="L136" t="n">
-        <v>1.82</v>
+        <v>2.29</v>
       </c>
       <c r="M136" t="inlineStr">
         <is>
-          <t>07/10/2023 15:49</t>
+          <t>07/10/2023 15:50</t>
         </is>
       </c>
       <c r="N136" t="n">
-        <v>3.81</v>
+        <v>3.27</v>
       </c>
       <c r="O136" t="inlineStr">
         <is>
@@ -12940,15 +12940,15 @@
         </is>
       </c>
       <c r="P136" t="n">
-        <v>3.61</v>
+        <v>3.37</v>
       </c>
       <c r="Q136" t="inlineStr">
         <is>
-          <t>07/10/2023 15:49</t>
+          <t>07/10/2023 15:46</t>
         </is>
       </c>
       <c r="R136" t="n">
-        <v>4.15</v>
+        <v>3.07</v>
       </c>
       <c r="S136" t="inlineStr">
         <is>
@@ -12956,16 +12956,16 @@
         </is>
       </c>
       <c r="T136" t="n">
-        <v>4.8</v>
+        <v>3.34</v>
       </c>
       <c r="U136" t="inlineStr">
         <is>
-          <t>07/10/2023 15:49</t>
+          <t>07/10/2023 15:50</t>
         </is>
       </c>
       <c r="V136" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/stevenage-wigan/6R47ZvWa/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/fleetwood-town-wycombe/QX6vW5P7/</t>
         </is>
       </c>
     </row>
@@ -13085,7 +13085,7 @@
       </c>
       <c r="F138" t="inlineStr">
         <is>
-          <t>Lincoln</t>
+          <t>Carlisle</t>
         </is>
       </c>
       <c r="G138" t="n">
@@ -13093,63 +13093,63 @@
       </c>
       <c r="H138" t="inlineStr">
         <is>
-          <t>Burton</t>
+          <t>Leyton Orient</t>
         </is>
       </c>
       <c r="I138" t="n">
         <v>1</v>
       </c>
       <c r="J138" t="n">
-        <v>1.85</v>
+        <v>2.38</v>
       </c>
       <c r="K138" t="inlineStr">
         <is>
-          <t>09/10/2023 20:11</t>
+          <t>07/10/2023 17:12</t>
         </is>
       </c>
       <c r="L138" t="n">
-        <v>2.07</v>
+        <v>2.72</v>
       </c>
       <c r="M138" t="inlineStr">
         <is>
-          <t>14/10/2023 15:58</t>
+          <t>14/10/2023 15:54</t>
         </is>
       </c>
       <c r="N138" t="n">
-        <v>3.6</v>
+        <v>3.22</v>
       </c>
       <c r="O138" t="inlineStr">
         <is>
-          <t>09/10/2023 20:11</t>
+          <t>07/10/2023 17:12</t>
         </is>
       </c>
       <c r="P138" t="n">
-        <v>3.38</v>
+        <v>3.34</v>
       </c>
       <c r="Q138" t="inlineStr">
         <is>
-          <t>14/10/2023 15:58</t>
+          <t>14/10/2023 15:54</t>
         </is>
       </c>
       <c r="R138" t="n">
-        <v>4.09</v>
+        <v>3.03</v>
       </c>
       <c r="S138" t="inlineStr">
         <is>
-          <t>09/10/2023 20:11</t>
+          <t>07/10/2023 17:12</t>
         </is>
       </c>
       <c r="T138" t="n">
-        <v>3.93</v>
+        <v>2.73</v>
       </c>
       <c r="U138" t="inlineStr">
         <is>
-          <t>14/10/2023 15:58</t>
+          <t>14/10/2023 15:52</t>
         </is>
       </c>
       <c r="V138" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/lincoln-city-burton/8fRxkKVn/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/carlisle-leyton-orient/lAp6ft8P/</t>
         </is>
       </c>
     </row>
@@ -13177,7 +13177,7 @@
       </c>
       <c r="F139" t="inlineStr">
         <is>
-          <t>Carlisle</t>
+          <t>Lincoln</t>
         </is>
       </c>
       <c r="G139" t="n">
@@ -13185,63 +13185,63 @@
       </c>
       <c r="H139" t="inlineStr">
         <is>
-          <t>Leyton Orient</t>
+          <t>Burton</t>
         </is>
       </c>
       <c r="I139" t="n">
         <v>1</v>
       </c>
       <c r="J139" t="n">
-        <v>2.38</v>
+        <v>1.85</v>
       </c>
       <c r="K139" t="inlineStr">
         <is>
-          <t>07/10/2023 17:12</t>
+          <t>09/10/2023 20:11</t>
         </is>
       </c>
       <c r="L139" t="n">
-        <v>2.72</v>
+        <v>2.07</v>
       </c>
       <c r="M139" t="inlineStr">
         <is>
-          <t>14/10/2023 15:54</t>
+          <t>14/10/2023 15:58</t>
         </is>
       </c>
       <c r="N139" t="n">
-        <v>3.22</v>
+        <v>3.6</v>
       </c>
       <c r="O139" t="inlineStr">
         <is>
-          <t>07/10/2023 17:12</t>
+          <t>09/10/2023 20:11</t>
         </is>
       </c>
       <c r="P139" t="n">
-        <v>3.34</v>
+        <v>3.38</v>
       </c>
       <c r="Q139" t="inlineStr">
         <is>
-          <t>14/10/2023 15:54</t>
+          <t>14/10/2023 15:58</t>
         </is>
       </c>
       <c r="R139" t="n">
-        <v>3.03</v>
+        <v>4.09</v>
       </c>
       <c r="S139" t="inlineStr">
         <is>
-          <t>07/10/2023 17:12</t>
+          <t>09/10/2023 20:11</t>
         </is>
       </c>
       <c r="T139" t="n">
-        <v>2.73</v>
+        <v>3.93</v>
       </c>
       <c r="U139" t="inlineStr">
         <is>
-          <t>14/10/2023 15:52</t>
+          <t>14/10/2023 15:58</t>
         </is>
       </c>
       <c r="V139" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/carlisle-leyton-orient/lAp6ft8P/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/lincoln-city-burton/8fRxkKVn/</t>
         </is>
       </c>
     </row>
@@ -14741,22 +14741,22 @@
       </c>
       <c r="F156" t="inlineStr">
         <is>
-          <t>Port Vale</t>
+          <t>Wycombe</t>
         </is>
       </c>
       <c r="G156" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H156" t="inlineStr">
         <is>
-          <t>Peterborough</t>
+          <t>Bolton</t>
         </is>
       </c>
       <c r="I156" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J156" t="n">
-        <v>2.98</v>
+        <v>2.88</v>
       </c>
       <c r="K156" t="inlineStr">
         <is>
@@ -14764,15 +14764,15 @@
         </is>
       </c>
       <c r="L156" t="n">
-        <v>3.31</v>
+        <v>2.56</v>
       </c>
       <c r="M156" t="inlineStr">
         <is>
-          <t>24/10/2023 20:29</t>
+          <t>24/10/2023 20:16</t>
         </is>
       </c>
       <c r="N156" t="n">
-        <v>3.37</v>
+        <v>3.36</v>
       </c>
       <c r="O156" t="inlineStr">
         <is>
@@ -14780,15 +14780,15 @@
         </is>
       </c>
       <c r="P156" t="n">
-        <v>3.6</v>
+        <v>3.48</v>
       </c>
       <c r="Q156" t="inlineStr">
         <is>
-          <t>24/10/2023 20:29</t>
+          <t>24/10/2023 20:16</t>
         </is>
       </c>
       <c r="R156" t="n">
-        <v>2.44</v>
+        <v>2.51</v>
       </c>
       <c r="S156" t="inlineStr">
         <is>
@@ -14796,16 +14796,16 @@
         </is>
       </c>
       <c r="T156" t="n">
-        <v>2.2</v>
+        <v>2.81</v>
       </c>
       <c r="U156" t="inlineStr">
         <is>
-          <t>24/10/2023 20:29</t>
+          <t>24/10/2023 20:16</t>
         </is>
       </c>
       <c r="V156" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/port-vale-peterborough/f9Ot5WLp/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/wycombe-bolton/xYmRCrui/</t>
         </is>
       </c>
     </row>
@@ -14833,7 +14833,7 @@
       </c>
       <c r="F157" t="inlineStr">
         <is>
-          <t>Wycombe</t>
+          <t>Northampton</t>
         </is>
       </c>
       <c r="G157" t="n">
@@ -14841,14 +14841,14 @@
       </c>
       <c r="H157" t="inlineStr">
         <is>
-          <t>Bolton</t>
+          <t>Leyton Orient</t>
         </is>
       </c>
       <c r="I157" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J157" t="n">
-        <v>2.88</v>
+        <v>2.21</v>
       </c>
       <c r="K157" t="inlineStr">
         <is>
@@ -14856,15 +14856,15 @@
         </is>
       </c>
       <c r="L157" t="n">
-        <v>2.56</v>
+        <v>2.58</v>
       </c>
       <c r="M157" t="inlineStr">
         <is>
-          <t>24/10/2023 20:16</t>
+          <t>24/10/2023 20:38</t>
         </is>
       </c>
       <c r="N157" t="n">
-        <v>3.36</v>
+        <v>3.32</v>
       </c>
       <c r="O157" t="inlineStr">
         <is>
@@ -14872,15 +14872,15 @@
         </is>
       </c>
       <c r="P157" t="n">
-        <v>3.48</v>
+        <v>3.14</v>
       </c>
       <c r="Q157" t="inlineStr">
         <is>
-          <t>24/10/2023 20:16</t>
+          <t>24/10/2023 20:38</t>
         </is>
       </c>
       <c r="R157" t="n">
-        <v>2.51</v>
+        <v>3.45</v>
       </c>
       <c r="S157" t="inlineStr">
         <is>
@@ -14888,16 +14888,16 @@
         </is>
       </c>
       <c r="T157" t="n">
-        <v>2.81</v>
+        <v>3.05</v>
       </c>
       <c r="U157" t="inlineStr">
         <is>
-          <t>24/10/2023 20:16</t>
+          <t>24/10/2023 20:04</t>
         </is>
       </c>
       <c r="V157" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/wycombe-bolton/xYmRCrui/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/northampton-leyton-orient/2HWE9CDT/</t>
         </is>
       </c>
     </row>
@@ -15017,22 +15017,22 @@
       </c>
       <c r="F159" t="inlineStr">
         <is>
-          <t>Northampton</t>
+          <t>Port Vale</t>
         </is>
       </c>
       <c r="G159" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H159" t="inlineStr">
         <is>
-          <t>Leyton Orient</t>
+          <t>Peterborough</t>
         </is>
       </c>
       <c r="I159" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J159" t="n">
-        <v>2.21</v>
+        <v>2.98</v>
       </c>
       <c r="K159" t="inlineStr">
         <is>
@@ -15040,15 +15040,15 @@
         </is>
       </c>
       <c r="L159" t="n">
-        <v>2.58</v>
+        <v>3.31</v>
       </c>
       <c r="M159" t="inlineStr">
         <is>
-          <t>24/10/2023 20:38</t>
+          <t>24/10/2023 20:29</t>
         </is>
       </c>
       <c r="N159" t="n">
-        <v>3.32</v>
+        <v>3.37</v>
       </c>
       <c r="O159" t="inlineStr">
         <is>
@@ -15056,15 +15056,15 @@
         </is>
       </c>
       <c r="P159" t="n">
-        <v>3.14</v>
+        <v>3.6</v>
       </c>
       <c r="Q159" t="inlineStr">
         <is>
-          <t>24/10/2023 20:38</t>
+          <t>24/10/2023 20:29</t>
         </is>
       </c>
       <c r="R159" t="n">
-        <v>3.45</v>
+        <v>2.44</v>
       </c>
       <c r="S159" t="inlineStr">
         <is>
@@ -15072,16 +15072,16 @@
         </is>
       </c>
       <c r="T159" t="n">
-        <v>3.05</v>
+        <v>2.2</v>
       </c>
       <c r="U159" t="inlineStr">
         <is>
-          <t>24/10/2023 20:04</t>
+          <t>24/10/2023 20:29</t>
         </is>
       </c>
       <c r="V159" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/northampton-leyton-orient/2HWE9CDT/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/port-vale-peterborough/f9Ot5WLp/</t>
         </is>
       </c>
     </row>
@@ -16213,22 +16213,22 @@
       </c>
       <c r="F172" t="inlineStr">
         <is>
-          <t>Charlton</t>
+          <t>Cambridge Utd</t>
         </is>
       </c>
       <c r="G172" t="n">
+        <v>1</v>
+      </c>
+      <c r="H172" t="inlineStr">
+        <is>
+          <t>Carlisle</t>
+        </is>
+      </c>
+      <c r="I172" t="n">
         <v>0</v>
       </c>
-      <c r="H172" t="inlineStr">
-        <is>
-          <t>Bolton</t>
-        </is>
-      </c>
-      <c r="I172" t="n">
-        <v>2</v>
-      </c>
       <c r="J172" t="n">
-        <v>2.47</v>
+        <v>2.04</v>
       </c>
       <c r="K172" t="inlineStr">
         <is>
@@ -16240,11 +16240,11 @@
       </c>
       <c r="M172" t="inlineStr">
         <is>
-          <t>28/10/2023 15:57</t>
+          <t>28/10/2023 13:34</t>
         </is>
       </c>
       <c r="N172" t="n">
-        <v>3.42</v>
+        <v>3.13</v>
       </c>
       <c r="O172" t="inlineStr">
         <is>
@@ -16252,15 +16252,15 @@
         </is>
       </c>
       <c r="P172" t="n">
-        <v>3.6</v>
+        <v>3.18</v>
       </c>
       <c r="Q172" t="inlineStr">
         <is>
-          <t>28/10/2023 15:57</t>
+          <t>28/10/2023 11:52</t>
         </is>
       </c>
       <c r="R172" t="n">
-        <v>2.89</v>
+        <v>3.96</v>
       </c>
       <c r="S172" t="inlineStr">
         <is>
@@ -16268,16 +16268,16 @@
         </is>
       </c>
       <c r="T172" t="n">
-        <v>2.9</v>
+        <v>3.27</v>
       </c>
       <c r="U172" t="inlineStr">
         <is>
-          <t>28/10/2023 15:57</t>
+          <t>28/10/2023 13:34</t>
         </is>
       </c>
       <c r="V172" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/charlton-bolton/OnBJkCwe/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/cambridge-utd-carlisle/Aq7FjhOl/</t>
         </is>
       </c>
     </row>
@@ -16673,22 +16673,22 @@
       </c>
       <c r="F177" t="inlineStr">
         <is>
-          <t>Cambridge Utd</t>
+          <t>Charlton</t>
         </is>
       </c>
       <c r="G177" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H177" t="inlineStr">
         <is>
-          <t>Carlisle</t>
+          <t>Bolton</t>
         </is>
       </c>
       <c r="I177" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J177" t="n">
-        <v>2.04</v>
+        <v>2.47</v>
       </c>
       <c r="K177" t="inlineStr">
         <is>
@@ -16700,11 +16700,11 @@
       </c>
       <c r="M177" t="inlineStr">
         <is>
-          <t>28/10/2023 13:34</t>
+          <t>28/10/2023 15:57</t>
         </is>
       </c>
       <c r="N177" t="n">
-        <v>3.13</v>
+        <v>3.42</v>
       </c>
       <c r="O177" t="inlineStr">
         <is>
@@ -16712,15 +16712,15 @@
         </is>
       </c>
       <c r="P177" t="n">
-        <v>3.18</v>
+        <v>3.6</v>
       </c>
       <c r="Q177" t="inlineStr">
         <is>
-          <t>28/10/2023 11:52</t>
+          <t>28/10/2023 15:57</t>
         </is>
       </c>
       <c r="R177" t="n">
-        <v>3.96</v>
+        <v>2.89</v>
       </c>
       <c r="S177" t="inlineStr">
         <is>
@@ -16728,16 +16728,16 @@
         </is>
       </c>
       <c r="T177" t="n">
-        <v>3.27</v>
+        <v>2.9</v>
       </c>
       <c r="U177" t="inlineStr">
         <is>
-          <t>28/10/2023 13:34</t>
+          <t>28/10/2023 15:57</t>
         </is>
       </c>
       <c r="V177" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/cambridge-utd-carlisle/Aq7FjhOl/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/charlton-bolton/OnBJkCwe/</t>
         </is>
       </c>
     </row>
@@ -16765,22 +16765,22 @@
       </c>
       <c r="F178" t="inlineStr">
         <is>
-          <t>Wycombe</t>
+          <t>Derby</t>
         </is>
       </c>
       <c r="G178" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H178" t="inlineStr">
         <is>
-          <t>Cambridge Utd</t>
+          <t>Northampton</t>
         </is>
       </c>
       <c r="I178" t="n">
         <v>0</v>
       </c>
       <c r="J178" t="n">
-        <v>1.83</v>
+        <v>1.61</v>
       </c>
       <c r="K178" t="inlineStr">
         <is>
@@ -16788,15 +16788,15 @@
         </is>
       </c>
       <c r="L178" t="n">
-        <v>1.76</v>
+        <v>1.57</v>
       </c>
       <c r="M178" t="inlineStr">
         <is>
-          <t>31/10/2023 20:43</t>
+          <t>31/10/2023 20:31</t>
         </is>
       </c>
       <c r="N178" t="n">
-        <v>3.68</v>
+        <v>3.85</v>
       </c>
       <c r="O178" t="inlineStr">
         <is>
@@ -16804,15 +16804,15 @@
         </is>
       </c>
       <c r="P178" t="n">
-        <v>3.83</v>
+        <v>3.85</v>
       </c>
       <c r="Q178" t="inlineStr">
         <is>
-          <t>31/10/2023 20:43</t>
+          <t>31/10/2023 20:44</t>
         </is>
       </c>
       <c r="R178" t="n">
-        <v>4.38</v>
+        <v>5.4</v>
       </c>
       <c r="S178" t="inlineStr">
         <is>
@@ -16820,16 +16820,16 @@
         </is>
       </c>
       <c r="T178" t="n">
-        <v>4.8</v>
+        <v>7.11</v>
       </c>
       <c r="U178" t="inlineStr">
         <is>
-          <t>31/10/2023 20:40</t>
+          <t>31/10/2023 20:44</t>
         </is>
       </c>
       <c r="V178" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/wycombe-cambridge-utd/48kvj6Fm/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/derby-northampton/0hvagK4r/</t>
         </is>
       </c>
     </row>
@@ -16857,22 +16857,22 @@
       </c>
       <c r="F179" t="inlineStr">
         <is>
-          <t>Derby</t>
+          <t>Lincoln</t>
         </is>
       </c>
       <c r="G179" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H179" t="inlineStr">
         <is>
-          <t>Northampton</t>
+          <t>Oxford Utd</t>
         </is>
       </c>
       <c r="I179" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J179" t="n">
-        <v>1.61</v>
+        <v>3.31</v>
       </c>
       <c r="K179" t="inlineStr">
         <is>
@@ -16880,15 +16880,15 @@
         </is>
       </c>
       <c r="L179" t="n">
-        <v>1.57</v>
+        <v>3.4</v>
       </c>
       <c r="M179" t="inlineStr">
         <is>
-          <t>31/10/2023 20:31</t>
+          <t>31/10/2023 20:16</t>
         </is>
       </c>
       <c r="N179" t="n">
-        <v>3.85</v>
+        <v>3.19</v>
       </c>
       <c r="O179" t="inlineStr">
         <is>
@@ -16896,15 +16896,15 @@
         </is>
       </c>
       <c r="P179" t="n">
-        <v>3.85</v>
+        <v>3.21</v>
       </c>
       <c r="Q179" t="inlineStr">
         <is>
-          <t>31/10/2023 20:44</t>
+          <t>31/10/2023 20:16</t>
         </is>
       </c>
       <c r="R179" t="n">
-        <v>5.4</v>
+        <v>2.25</v>
       </c>
       <c r="S179" t="inlineStr">
         <is>
@@ -16912,16 +16912,16 @@
         </is>
       </c>
       <c r="T179" t="n">
-        <v>7.11</v>
+        <v>2.34</v>
       </c>
       <c r="U179" t="inlineStr">
         <is>
-          <t>31/10/2023 20:44</t>
+          <t>31/10/2023 20:16</t>
         </is>
       </c>
       <c r="V179" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/derby-northampton/0hvagK4r/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/lincoln-city-oxford-utd/zBWBjIl1/</t>
         </is>
       </c>
     </row>
@@ -16949,22 +16949,22 @@
       </c>
       <c r="F180" t="inlineStr">
         <is>
-          <t>Lincoln</t>
+          <t>Wigan</t>
         </is>
       </c>
       <c r="G180" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H180" t="inlineStr">
         <is>
-          <t>Oxford Utd</t>
+          <t>Charlton</t>
         </is>
       </c>
       <c r="I180" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J180" t="n">
-        <v>3.31</v>
+        <v>2.49</v>
       </c>
       <c r="K180" t="inlineStr">
         <is>
@@ -16972,15 +16972,15 @@
         </is>
       </c>
       <c r="L180" t="n">
-        <v>3.4</v>
+        <v>2.35</v>
       </c>
       <c r="M180" t="inlineStr">
         <is>
-          <t>31/10/2023 20:16</t>
+          <t>31/10/2023 20:29</t>
         </is>
       </c>
       <c r="N180" t="n">
-        <v>3.19</v>
+        <v>3.5</v>
       </c>
       <c r="O180" t="inlineStr">
         <is>
@@ -16988,15 +16988,15 @@
         </is>
       </c>
       <c r="P180" t="n">
-        <v>3.21</v>
+        <v>3.68</v>
       </c>
       <c r="Q180" t="inlineStr">
         <is>
-          <t>31/10/2023 20:16</t>
+          <t>31/10/2023 20:29</t>
         </is>
       </c>
       <c r="R180" t="n">
-        <v>2.25</v>
+        <v>2.81</v>
       </c>
       <c r="S180" t="inlineStr">
         <is>
@@ -17004,16 +17004,16 @@
         </is>
       </c>
       <c r="T180" t="n">
-        <v>2.34</v>
+        <v>2.98</v>
       </c>
       <c r="U180" t="inlineStr">
         <is>
-          <t>31/10/2023 20:16</t>
+          <t>31/10/2023 20:29</t>
         </is>
       </c>
       <c r="V180" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/lincoln-city-oxford-utd/zBWBjIl1/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/wigan-charlton/Mq0Zjn0s/</t>
         </is>
       </c>
     </row>
@@ -17041,22 +17041,22 @@
       </c>
       <c r="F181" t="inlineStr">
         <is>
-          <t>Wigan</t>
+          <t>Wycombe</t>
         </is>
       </c>
       <c r="G181" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H181" t="inlineStr">
         <is>
-          <t>Charlton</t>
+          <t>Cambridge Utd</t>
         </is>
       </c>
       <c r="I181" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J181" t="n">
-        <v>2.49</v>
+        <v>1.83</v>
       </c>
       <c r="K181" t="inlineStr">
         <is>
@@ -17064,15 +17064,15 @@
         </is>
       </c>
       <c r="L181" t="n">
-        <v>2.35</v>
+        <v>1.76</v>
       </c>
       <c r="M181" t="inlineStr">
         <is>
-          <t>31/10/2023 20:29</t>
+          <t>31/10/2023 20:43</t>
         </is>
       </c>
       <c r="N181" t="n">
-        <v>3.5</v>
+        <v>3.68</v>
       </c>
       <c r="O181" t="inlineStr">
         <is>
@@ -17080,15 +17080,15 @@
         </is>
       </c>
       <c r="P181" t="n">
-        <v>3.68</v>
+        <v>3.83</v>
       </c>
       <c r="Q181" t="inlineStr">
         <is>
-          <t>31/10/2023 20:29</t>
+          <t>31/10/2023 20:43</t>
         </is>
       </c>
       <c r="R181" t="n">
-        <v>2.81</v>
+        <v>4.38</v>
       </c>
       <c r="S181" t="inlineStr">
         <is>
@@ -17096,16 +17096,16 @@
         </is>
       </c>
       <c r="T181" t="n">
-        <v>2.98</v>
+        <v>4.8</v>
       </c>
       <c r="U181" t="inlineStr">
         <is>
-          <t>31/10/2023 20:29</t>
+          <t>31/10/2023 20:40</t>
         </is>
       </c>
       <c r="V181" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/wigan-charlton/Mq0Zjn0s/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/wycombe-cambridge-utd/48kvj6Fm/</t>
         </is>
       </c>
     </row>
@@ -17198,6 +17198,190 @@
       <c r="V182" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/england/league-one/fleetwood-town-blackpool/dKX7ibZf/</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" s="1" t="n">
+        <v>182</v>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>england</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>league-one</t>
+        </is>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E183" s="2" t="n">
+        <v>45237.86458333334</v>
+      </c>
+      <c r="F183" t="inlineStr">
+        <is>
+          <t>Wigan</t>
+        </is>
+      </c>
+      <c r="G183" t="n">
+        <v>2</v>
+      </c>
+      <c r="H183" t="inlineStr">
+        <is>
+          <t>Peterborough</t>
+        </is>
+      </c>
+      <c r="I183" t="n">
+        <v>1</v>
+      </c>
+      <c r="J183" t="n">
+        <v>3.29</v>
+      </c>
+      <c r="K183" t="inlineStr">
+        <is>
+          <t>05/11/2023 19:43</t>
+        </is>
+      </c>
+      <c r="L183" t="n">
+        <v>3.07</v>
+      </c>
+      <c r="M183" t="inlineStr">
+        <is>
+          <t>07/11/2023 20:43</t>
+        </is>
+      </c>
+      <c r="N183" t="n">
+        <v>3.42</v>
+      </c>
+      <c r="O183" t="inlineStr">
+        <is>
+          <t>05/11/2023 19:43</t>
+        </is>
+      </c>
+      <c r="P183" t="n">
+        <v>3.76</v>
+      </c>
+      <c r="Q183" t="inlineStr">
+        <is>
+          <t>07/11/2023 20:43</t>
+        </is>
+      </c>
+      <c r="R183" t="n">
+        <v>2.24</v>
+      </c>
+      <c r="S183" t="inlineStr">
+        <is>
+          <t>05/11/2023 19:43</t>
+        </is>
+      </c>
+      <c r="T183" t="n">
+        <v>2.27</v>
+      </c>
+      <c r="U183" t="inlineStr">
+        <is>
+          <t>07/11/2023 20:42</t>
+        </is>
+      </c>
+      <c r="V183" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/england/league-one/wigan-peterborough/GQDgoxVB/</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" s="1" t="n">
+        <v>183</v>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>england</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>league-one</t>
+        </is>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E184" s="2" t="n">
+        <v>45237.86458333334</v>
+      </c>
+      <c r="F184" t="inlineStr">
+        <is>
+          <t>Shrewsbury</t>
+        </is>
+      </c>
+      <c r="G184" t="n">
+        <v>0</v>
+      </c>
+      <c r="H184" t="inlineStr">
+        <is>
+          <t>Bolton</t>
+        </is>
+      </c>
+      <c r="I184" t="n">
+        <v>2</v>
+      </c>
+      <c r="J184" t="n">
+        <v>3.58</v>
+      </c>
+      <c r="K184" t="inlineStr">
+        <is>
+          <t>31/10/2023 07:11</t>
+        </is>
+      </c>
+      <c r="L184" t="n">
+        <v>3.93</v>
+      </c>
+      <c r="M184" t="inlineStr">
+        <is>
+          <t>07/11/2023 20:43</t>
+        </is>
+      </c>
+      <c r="N184" t="n">
+        <v>3.37</v>
+      </c>
+      <c r="O184" t="inlineStr">
+        <is>
+          <t>31/10/2023 07:11</t>
+        </is>
+      </c>
+      <c r="P184" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="Q184" t="inlineStr">
+        <is>
+          <t>07/11/2023 20:43</t>
+        </is>
+      </c>
+      <c r="R184" t="n">
+        <v>2.14</v>
+      </c>
+      <c r="S184" t="inlineStr">
+        <is>
+          <t>31/10/2023 07:11</t>
+        </is>
+      </c>
+      <c r="T184" t="n">
+        <v>2.02</v>
+      </c>
+      <c r="U184" t="inlineStr">
+        <is>
+          <t>07/11/2023 20:43</t>
+        </is>
+      </c>
+      <c r="V184" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/england/league-one/shrewsbury-bolton/Qaa4d8xK/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 21-11-2023 20:45
</commit_message>
<xml_diff>
--- a/2023/england_league-one_2023-2024.xlsx
+++ b/2023/england_league-one_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V199"/>
+  <dimension ref="A1:V200"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8945,71 +8945,71 @@
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>Oxford Utd</t>
+          <t>Northampton</t>
         </is>
       </c>
       <c r="G93" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H93" t="inlineStr">
         <is>
-          <t>Exeter</t>
+          <t>Barnsley</t>
         </is>
       </c>
       <c r="I93" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J93" t="n">
-        <v>1.79</v>
+        <v>2.63</v>
       </c>
       <c r="K93" t="inlineStr">
         <is>
-          <t>16/09/2023 17:13</t>
+          <t>19/09/2023 20:12</t>
         </is>
       </c>
       <c r="L93" t="n">
-        <v>1.81</v>
+        <v>2.9</v>
       </c>
       <c r="M93" t="inlineStr">
         <is>
-          <t>23/09/2023 15:31</t>
+          <t>23/09/2023 15:56</t>
         </is>
       </c>
       <c r="N93" t="n">
-        <v>3.75</v>
+        <v>3.4</v>
       </c>
       <c r="O93" t="inlineStr">
         <is>
-          <t>16/09/2023 17:13</t>
+          <t>19/09/2023 20:12</t>
         </is>
       </c>
       <c r="P93" t="n">
-        <v>3.79</v>
+        <v>3.36</v>
       </c>
       <c r="Q93" t="inlineStr">
         <is>
-          <t>23/09/2023 15:31</t>
+          <t>23/09/2023 15:33</t>
         </is>
       </c>
       <c r="R93" t="n">
-        <v>4.56</v>
+        <v>2.6</v>
       </c>
       <c r="S93" t="inlineStr">
         <is>
-          <t>16/09/2023 17:13</t>
+          <t>19/09/2023 20:12</t>
         </is>
       </c>
       <c r="T93" t="n">
-        <v>4.56</v>
+        <v>2.56</v>
       </c>
       <c r="U93" t="inlineStr">
         <is>
-          <t>23/09/2023 15:31</t>
+          <t>23/09/2023 15:56</t>
         </is>
       </c>
       <c r="V93" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/oxford-utd-exeter/hCAxehcp/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/northampton-barnsley/nVX9aYlT/</t>
         </is>
       </c>
     </row>
@@ -9221,71 +9221,71 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>Northampton</t>
+          <t>Oxford Utd</t>
         </is>
       </c>
       <c r="G96" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>Barnsley</t>
+          <t>Exeter</t>
         </is>
       </c>
       <c r="I96" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J96" t="n">
-        <v>2.63</v>
+        <v>1.79</v>
       </c>
       <c r="K96" t="inlineStr">
         <is>
-          <t>19/09/2023 20:12</t>
+          <t>16/09/2023 17:13</t>
         </is>
       </c>
       <c r="L96" t="n">
-        <v>2.9</v>
+        <v>1.81</v>
       </c>
       <c r="M96" t="inlineStr">
         <is>
-          <t>23/09/2023 15:56</t>
+          <t>23/09/2023 15:31</t>
         </is>
       </c>
       <c r="N96" t="n">
-        <v>3.4</v>
+        <v>3.75</v>
       </c>
       <c r="O96" t="inlineStr">
         <is>
-          <t>19/09/2023 20:12</t>
+          <t>16/09/2023 17:13</t>
         </is>
       </c>
       <c r="P96" t="n">
-        <v>3.36</v>
+        <v>3.79</v>
       </c>
       <c r="Q96" t="inlineStr">
         <is>
-          <t>23/09/2023 15:33</t>
+          <t>23/09/2023 15:31</t>
         </is>
       </c>
       <c r="R96" t="n">
-        <v>2.6</v>
+        <v>4.56</v>
       </c>
       <c r="S96" t="inlineStr">
         <is>
-          <t>19/09/2023 20:12</t>
+          <t>16/09/2023 17:13</t>
         </is>
       </c>
       <c r="T96" t="n">
-        <v>2.56</v>
+        <v>4.56</v>
       </c>
       <c r="U96" t="inlineStr">
         <is>
-          <t>23/09/2023 15:56</t>
+          <t>23/09/2023 15:31</t>
         </is>
       </c>
       <c r="V96" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/northampton-barnsley/nVX9aYlT/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/oxford-utd-exeter/hCAxehcp/</t>
         </is>
       </c>
     </row>
@@ -9681,71 +9681,71 @@
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>Bristol Rovers</t>
+          <t>Burton</t>
         </is>
       </c>
       <c r="G101" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H101" t="inlineStr">
         <is>
-          <t>Wigan</t>
+          <t>Fleetwood</t>
         </is>
       </c>
       <c r="I101" t="n">
         <v>1</v>
       </c>
       <c r="J101" t="n">
-        <v>2.21</v>
+        <v>2.2</v>
       </c>
       <c r="K101" t="inlineStr">
         <is>
-          <t>19/09/2023 16:12</t>
+          <t>19/09/2023 20:12</t>
         </is>
       </c>
       <c r="L101" t="n">
-        <v>2.23</v>
+        <v>2.81</v>
       </c>
       <c r="M101" t="inlineStr">
         <is>
-          <t>23/09/2023 15:48</t>
+          <t>23/09/2023 15:37</t>
         </is>
       </c>
       <c r="N101" t="n">
-        <v>3.46</v>
+        <v>3.41</v>
       </c>
       <c r="O101" t="inlineStr">
         <is>
-          <t>19/09/2023 16:12</t>
+          <t>19/09/2023 20:12</t>
         </is>
       </c>
       <c r="P101" t="n">
-        <v>3.6</v>
+        <v>3.44</v>
       </c>
       <c r="Q101" t="inlineStr">
         <is>
-          <t>23/09/2023 15:37</t>
+          <t>23/09/2023 15:46</t>
         </is>
       </c>
       <c r="R101" t="n">
-        <v>3.14</v>
+        <v>3.38</v>
       </c>
       <c r="S101" t="inlineStr">
         <is>
-          <t>19/09/2023 16:12</t>
+          <t>19/09/2023 20:12</t>
         </is>
       </c>
       <c r="T101" t="n">
-        <v>3.26</v>
+        <v>2.58</v>
       </c>
       <c r="U101" t="inlineStr">
         <is>
-          <t>23/09/2023 15:48</t>
+          <t>23/09/2023 15:46</t>
         </is>
       </c>
       <c r="V101" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/bristol-rovers-wigan/WYws6I5o/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/burton-fleetwood-town/APxo5xLi/</t>
         </is>
       </c>
     </row>
@@ -9773,71 +9773,71 @@
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>Burton</t>
+          <t>Bristol Rovers</t>
         </is>
       </c>
       <c r="G102" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H102" t="inlineStr">
         <is>
-          <t>Fleetwood</t>
+          <t>Wigan</t>
         </is>
       </c>
       <c r="I102" t="n">
         <v>1</v>
       </c>
       <c r="J102" t="n">
-        <v>2.2</v>
+        <v>2.21</v>
       </c>
       <c r="K102" t="inlineStr">
         <is>
-          <t>19/09/2023 20:12</t>
+          <t>19/09/2023 16:12</t>
         </is>
       </c>
       <c r="L102" t="n">
-        <v>2.81</v>
+        <v>2.23</v>
       </c>
       <c r="M102" t="inlineStr">
         <is>
+          <t>23/09/2023 15:48</t>
+        </is>
+      </c>
+      <c r="N102" t="n">
+        <v>3.46</v>
+      </c>
+      <c r="O102" t="inlineStr">
+        <is>
+          <t>19/09/2023 16:12</t>
+        </is>
+      </c>
+      <c r="P102" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="Q102" t="inlineStr">
+        <is>
           <t>23/09/2023 15:37</t>
         </is>
       </c>
-      <c r="N102" t="n">
-        <v>3.41</v>
-      </c>
-      <c r="O102" t="inlineStr">
-        <is>
-          <t>19/09/2023 20:12</t>
-        </is>
-      </c>
-      <c r="P102" t="n">
-        <v>3.44</v>
-      </c>
-      <c r="Q102" t="inlineStr">
-        <is>
-          <t>23/09/2023 15:46</t>
-        </is>
-      </c>
       <c r="R102" t="n">
-        <v>3.38</v>
+        <v>3.14</v>
       </c>
       <c r="S102" t="inlineStr">
         <is>
-          <t>19/09/2023 20:12</t>
+          <t>19/09/2023 16:12</t>
         </is>
       </c>
       <c r="T102" t="n">
-        <v>2.58</v>
+        <v>3.26</v>
       </c>
       <c r="U102" t="inlineStr">
         <is>
-          <t>23/09/2023 15:46</t>
+          <t>23/09/2023 15:48</t>
         </is>
       </c>
       <c r="V102" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/burton-fleetwood-town/APxo5xLi/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/bristol-rovers-wigan/WYws6I5o/</t>
         </is>
       </c>
     </row>
@@ -9865,22 +9865,22 @@
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>Wycombe</t>
+          <t>Reading</t>
         </is>
       </c>
       <c r="G103" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H103" t="inlineStr">
         <is>
-          <t>Carlisle</t>
+          <t>Burton</t>
         </is>
       </c>
       <c r="I103" t="n">
         <v>0</v>
       </c>
       <c r="J103" t="n">
-        <v>1.78</v>
+        <v>2</v>
       </c>
       <c r="K103" t="inlineStr">
         <is>
@@ -9888,15 +9888,15 @@
         </is>
       </c>
       <c r="L103" t="n">
-        <v>1.96</v>
+        <v>1.92</v>
       </c>
       <c r="M103" t="inlineStr">
         <is>
-          <t>30/09/2023 15:51</t>
+          <t>30/09/2023 15:57</t>
         </is>
       </c>
       <c r="N103" t="n">
-        <v>3.7</v>
+        <v>3.32</v>
       </c>
       <c r="O103" t="inlineStr">
         <is>
@@ -9904,15 +9904,15 @@
         </is>
       </c>
       <c r="P103" t="n">
-        <v>3.41</v>
+        <v>3.8</v>
       </c>
       <c r="Q103" t="inlineStr">
         <is>
-          <t>30/09/2023 15:51</t>
+          <t>30/09/2023 15:57</t>
         </is>
       </c>
       <c r="R103" t="n">
-        <v>4.31</v>
+        <v>3.82</v>
       </c>
       <c r="S103" t="inlineStr">
         <is>
@@ -9920,16 +9920,16 @@
         </is>
       </c>
       <c r="T103" t="n">
-        <v>4.31</v>
+        <v>4</v>
       </c>
       <c r="U103" t="inlineStr">
         <is>
-          <t>30/09/2023 15:51</t>
+          <t>30/09/2023 15:57</t>
         </is>
       </c>
       <c r="V103" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/wycombe-carlisle/YuV9Uhl3/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/reading-burton/WGlF8BRq/</t>
         </is>
       </c>
     </row>
@@ -9957,22 +9957,22 @@
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>Wigan</t>
+          <t>Barnsley</t>
         </is>
       </c>
       <c r="G104" t="n">
+        <v>0</v>
+      </c>
+      <c r="H104" t="inlineStr">
+        <is>
+          <t>Blackpool</t>
+        </is>
+      </c>
+      <c r="I104" t="n">
         <v>1</v>
       </c>
-      <c r="H104" t="inlineStr">
-        <is>
-          <t>Portsmouth</t>
-        </is>
-      </c>
-      <c r="I104" t="n">
-        <v>2</v>
-      </c>
       <c r="J104" t="n">
-        <v>3.14</v>
+        <v>2.18</v>
       </c>
       <c r="K104" t="inlineStr">
         <is>
@@ -9980,15 +9980,15 @@
         </is>
       </c>
       <c r="L104" t="n">
-        <v>3.11</v>
+        <v>2.51</v>
       </c>
       <c r="M104" t="inlineStr">
         <is>
-          <t>30/09/2023 14:21</t>
+          <t>30/09/2023 15:50</t>
         </is>
       </c>
       <c r="N104" t="n">
-        <v>3.21</v>
+        <v>3.31</v>
       </c>
       <c r="O104" t="inlineStr">
         <is>
@@ -9996,15 +9996,15 @@
         </is>
       </c>
       <c r="P104" t="n">
-        <v>3.59</v>
+        <v>3.6</v>
       </c>
       <c r="Q104" t="inlineStr">
         <is>
-          <t>30/09/2023 15:38</t>
+          <t>30/09/2023 15:50</t>
         </is>
       </c>
       <c r="R104" t="n">
-        <v>2.42</v>
+        <v>3.55</v>
       </c>
       <c r="S104" t="inlineStr">
         <is>
@@ -10012,16 +10012,16 @@
         </is>
       </c>
       <c r="T104" t="n">
-        <v>2.31</v>
+        <v>2.81</v>
       </c>
       <c r="U104" t="inlineStr">
         <is>
-          <t>30/09/2023 14:21</t>
+          <t>30/09/2023 15:51</t>
         </is>
       </c>
       <c r="V104" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/wigan-portsmouth/KxR5VYYd/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/barnsley-blackpool/40HNIeki/</t>
         </is>
       </c>
     </row>
@@ -10049,71 +10049,71 @@
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>Stevenage</t>
+          <t>Derby</t>
         </is>
       </c>
       <c r="G105" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H105" t="inlineStr">
         <is>
-          <t>Oxford Utd</t>
+          <t>Cambridge Utd</t>
         </is>
       </c>
       <c r="I105" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J105" t="n">
-        <v>2.53</v>
+        <v>1.56</v>
       </c>
       <c r="K105" t="inlineStr">
         <is>
-          <t>24/09/2023 03:13</t>
+          <t>23/09/2023 17:13</t>
         </is>
       </c>
       <c r="L105" t="n">
-        <v>2.42</v>
+        <v>1.64</v>
       </c>
       <c r="M105" t="inlineStr">
         <is>
-          <t>30/09/2023 15:51</t>
+          <t>30/09/2023 15:58</t>
         </is>
       </c>
       <c r="N105" t="n">
-        <v>3.2</v>
+        <v>4.18</v>
       </c>
       <c r="O105" t="inlineStr">
         <is>
-          <t>24/09/2023 03:13</t>
+          <t>23/09/2023 17:13</t>
         </is>
       </c>
       <c r="P105" t="n">
-        <v>3.42</v>
+        <v>4.2</v>
       </c>
       <c r="Q105" t="inlineStr">
         <is>
-          <t>30/09/2023 15:51</t>
+          <t>30/09/2023 15:58</t>
         </is>
       </c>
       <c r="R105" t="n">
-        <v>2.83</v>
+        <v>5.3</v>
       </c>
       <c r="S105" t="inlineStr">
         <is>
-          <t>24/09/2023 03:13</t>
+          <t>23/09/2023 17:13</t>
         </is>
       </c>
       <c r="T105" t="n">
-        <v>3.06</v>
+        <v>5.29</v>
       </c>
       <c r="U105" t="inlineStr">
         <is>
-          <t>30/09/2023 15:51</t>
+          <t>30/09/2023 15:58</t>
         </is>
       </c>
       <c r="V105" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/stevenage-oxford-utd/IXnN6kdd/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/derby-cambridge-utd/riGRHF4c/</t>
         </is>
       </c>
     </row>
@@ -10141,7 +10141,7 @@
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>Shrewsbury</t>
+          <t>Exeter</t>
         </is>
       </c>
       <c r="G106" t="n">
@@ -10149,63 +10149,63 @@
       </c>
       <c r="H106" t="inlineStr">
         <is>
-          <t>Charlton</t>
+          <t>Northampton</t>
         </is>
       </c>
       <c r="I106" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J106" t="n">
-        <v>2.67</v>
+        <v>1.73</v>
       </c>
       <c r="K106" t="inlineStr">
         <is>
-          <t>23/09/2023 17:13</t>
+          <t>24/09/2023 03:13</t>
         </is>
       </c>
       <c r="L106" t="n">
-        <v>3.08</v>
+        <v>2.13</v>
       </c>
       <c r="M106" t="inlineStr">
         <is>
-          <t>30/09/2023 15:57</t>
+          <t>30/09/2023 15:51</t>
         </is>
       </c>
       <c r="N106" t="n">
-        <v>3.15</v>
+        <v>3.48</v>
       </c>
       <c r="O106" t="inlineStr">
         <is>
-          <t>23/09/2023 17:13</t>
+          <t>24/09/2023 03:13</t>
         </is>
       </c>
       <c r="P106" t="n">
-        <v>3.43</v>
+        <v>3.53</v>
       </c>
       <c r="Q106" t="inlineStr">
         <is>
-          <t>30/09/2023 15:18</t>
+          <t>30/09/2023 15:51</t>
         </is>
       </c>
       <c r="R106" t="n">
-        <v>2.71</v>
+        <v>5.01</v>
       </c>
       <c r="S106" t="inlineStr">
         <is>
-          <t>23/09/2023 17:13</t>
+          <t>24/09/2023 03:13</t>
         </is>
       </c>
       <c r="T106" t="n">
-        <v>2.4</v>
+        <v>3.57</v>
       </c>
       <c r="U106" t="inlineStr">
         <is>
-          <t>30/09/2023 15:57</t>
+          <t>30/09/2023 15:51</t>
         </is>
       </c>
       <c r="V106" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/shrewsbury-charlton/vslJ7Vtj/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/exeter-northampton/0SAWGZJ3/</t>
         </is>
       </c>
     </row>
@@ -10233,22 +10233,22 @@
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>Reading</t>
+          <t>Fleetwood</t>
         </is>
       </c>
       <c r="G107" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H107" t="inlineStr">
         <is>
-          <t>Burton</t>
+          <t>Leyton Orient</t>
         </is>
       </c>
       <c r="I107" t="n">
         <v>0</v>
       </c>
       <c r="J107" t="n">
-        <v>2</v>
+        <v>2.16</v>
       </c>
       <c r="K107" t="inlineStr">
         <is>
@@ -10256,15 +10256,15 @@
         </is>
       </c>
       <c r="L107" t="n">
-        <v>1.92</v>
+        <v>2.23</v>
       </c>
       <c r="M107" t="inlineStr">
         <is>
-          <t>30/09/2023 15:57</t>
+          <t>30/09/2023 15:50</t>
         </is>
       </c>
       <c r="N107" t="n">
-        <v>3.32</v>
+        <v>3.36</v>
       </c>
       <c r="O107" t="inlineStr">
         <is>
@@ -10272,15 +10272,15 @@
         </is>
       </c>
       <c r="P107" t="n">
-        <v>3.8</v>
+        <v>3.48</v>
       </c>
       <c r="Q107" t="inlineStr">
         <is>
-          <t>30/09/2023 15:57</t>
+          <t>30/09/2023 15:50</t>
         </is>
       </c>
       <c r="R107" t="n">
-        <v>3.82</v>
+        <v>3.34</v>
       </c>
       <c r="S107" t="inlineStr">
         <is>
@@ -10288,16 +10288,16 @@
         </is>
       </c>
       <c r="T107" t="n">
-        <v>4</v>
+        <v>3.36</v>
       </c>
       <c r="U107" t="inlineStr">
         <is>
-          <t>30/09/2023 15:57</t>
+          <t>30/09/2023 15:50</t>
         </is>
       </c>
       <c r="V107" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/reading-burton/WGlF8BRq/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/fleetwood-town-leyton-orient/vJ9zGgZ9/</t>
         </is>
       </c>
     </row>
@@ -10325,22 +10325,22 @@
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>Port Vale</t>
+          <t>Lincoln</t>
         </is>
       </c>
       <c r="G108" t="n">
+        <v>2</v>
+      </c>
+      <c r="H108" t="inlineStr">
+        <is>
+          <t>Cheltenham</t>
+        </is>
+      </c>
+      <c r="I108" t="n">
         <v>0</v>
       </c>
-      <c r="H108" t="inlineStr">
-        <is>
-          <t>Bolton</t>
-        </is>
-      </c>
-      <c r="I108" t="n">
-        <v>1</v>
-      </c>
       <c r="J108" t="n">
-        <v>3.09</v>
+        <v>1.81</v>
       </c>
       <c r="K108" t="inlineStr">
         <is>
@@ -10348,48 +10348,48 @@
         </is>
       </c>
       <c r="L108" t="n">
-        <v>2.64</v>
+        <v>1.76</v>
       </c>
       <c r="M108" t="inlineStr">
         <is>
+          <t>30/09/2023 15:39</t>
+        </is>
+      </c>
+      <c r="N108" t="n">
+        <v>3.55</v>
+      </c>
+      <c r="O108" t="inlineStr">
+        <is>
+          <t>23/09/2023 17:13</t>
+        </is>
+      </c>
+      <c r="P108" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="Q108" t="inlineStr">
+        <is>
           <t>30/09/2023 15:48</t>
         </is>
       </c>
-      <c r="N108" t="n">
-        <v>3.23</v>
-      </c>
-      <c r="O108" t="inlineStr">
+      <c r="R108" t="n">
+        <v>4.74</v>
+      </c>
+      <c r="S108" t="inlineStr">
         <is>
           <t>23/09/2023 17:13</t>
         </is>
       </c>
-      <c r="P108" t="n">
-        <v>3.49</v>
-      </c>
-      <c r="Q108" t="inlineStr">
-        <is>
-          <t>30/09/2023 15:48</t>
-        </is>
-      </c>
-      <c r="R108" t="n">
-        <v>2.44</v>
-      </c>
-      <c r="S108" t="inlineStr">
-        <is>
-          <t>23/09/2023 17:13</t>
-        </is>
-      </c>
       <c r="T108" t="n">
-        <v>2.72</v>
+        <v>5.02</v>
       </c>
       <c r="U108" t="inlineStr">
         <is>
-          <t>30/09/2023 15:48</t>
+          <t>30/09/2023 15:40</t>
         </is>
       </c>
       <c r="V108" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/port-vale-bolton/U72mDiJS/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/lincoln-city-cheltenham/Yu9vFDlG/</t>
         </is>
       </c>
     </row>
@@ -10417,7 +10417,7 @@
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>Lincoln</t>
+          <t>Peterborough</t>
         </is>
       </c>
       <c r="G109" t="n">
@@ -10425,14 +10425,14 @@
       </c>
       <c r="H109" t="inlineStr">
         <is>
-          <t>Cheltenham</t>
+          <t>Bristol Rovers</t>
         </is>
       </c>
       <c r="I109" t="n">
         <v>0</v>
       </c>
       <c r="J109" t="n">
-        <v>1.81</v>
+        <v>1.77</v>
       </c>
       <c r="K109" t="inlineStr">
         <is>
@@ -10440,15 +10440,15 @@
         </is>
       </c>
       <c r="L109" t="n">
-        <v>1.76</v>
+        <v>1.83</v>
       </c>
       <c r="M109" t="inlineStr">
         <is>
-          <t>30/09/2023 15:39</t>
+          <t>30/09/2023 15:52</t>
         </is>
       </c>
       <c r="N109" t="n">
-        <v>3.55</v>
+        <v>3.96</v>
       </c>
       <c r="O109" t="inlineStr">
         <is>
@@ -10456,15 +10456,15 @@
         </is>
       </c>
       <c r="P109" t="n">
-        <v>3.7</v>
+        <v>3.97</v>
       </c>
       <c r="Q109" t="inlineStr">
         <is>
-          <t>30/09/2023 15:48</t>
+          <t>30/09/2023 15:52</t>
         </is>
       </c>
       <c r="R109" t="n">
-        <v>4.74</v>
+        <v>4.05</v>
       </c>
       <c r="S109" t="inlineStr">
         <is>
@@ -10472,16 +10472,16 @@
         </is>
       </c>
       <c r="T109" t="n">
-        <v>5.02</v>
+        <v>4.23</v>
       </c>
       <c r="U109" t="inlineStr">
         <is>
-          <t>30/09/2023 15:40</t>
+          <t>30/09/2023 15:52</t>
         </is>
       </c>
       <c r="V109" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/lincoln-city-cheltenham/Yu9vFDlG/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/peterborough-bristol-rovers/nqDrEX3M/</t>
         </is>
       </c>
     </row>
@@ -10509,71 +10509,71 @@
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>Fleetwood</t>
+          <t>Port Vale</t>
         </is>
       </c>
       <c r="G110" t="n">
+        <v>0</v>
+      </c>
+      <c r="H110" t="inlineStr">
+        <is>
+          <t>Bolton</t>
+        </is>
+      </c>
+      <c r="I110" t="n">
         <v>1</v>
       </c>
-      <c r="H110" t="inlineStr">
-        <is>
-          <t>Leyton Orient</t>
-        </is>
-      </c>
-      <c r="I110" t="n">
-        <v>0</v>
-      </c>
       <c r="J110" t="n">
-        <v>2.16</v>
+        <v>3.09</v>
       </c>
       <c r="K110" t="inlineStr">
         <is>
-          <t>24/09/2023 03:13</t>
+          <t>23/09/2023 17:13</t>
         </is>
       </c>
       <c r="L110" t="n">
-        <v>2.23</v>
+        <v>2.64</v>
       </c>
       <c r="M110" t="inlineStr">
         <is>
-          <t>30/09/2023 15:50</t>
+          <t>30/09/2023 15:48</t>
         </is>
       </c>
       <c r="N110" t="n">
-        <v>3.36</v>
+        <v>3.23</v>
       </c>
       <c r="O110" t="inlineStr">
         <is>
-          <t>24/09/2023 03:13</t>
+          <t>23/09/2023 17:13</t>
         </is>
       </c>
       <c r="P110" t="n">
-        <v>3.48</v>
+        <v>3.49</v>
       </c>
       <c r="Q110" t="inlineStr">
         <is>
-          <t>30/09/2023 15:50</t>
+          <t>30/09/2023 15:48</t>
         </is>
       </c>
       <c r="R110" t="n">
-        <v>3.34</v>
+        <v>2.44</v>
       </c>
       <c r="S110" t="inlineStr">
         <is>
-          <t>24/09/2023 03:13</t>
+          <t>23/09/2023 17:13</t>
         </is>
       </c>
       <c r="T110" t="n">
-        <v>3.36</v>
+        <v>2.72</v>
       </c>
       <c r="U110" t="inlineStr">
         <is>
-          <t>30/09/2023 15:50</t>
+          <t>30/09/2023 15:48</t>
         </is>
       </c>
       <c r="V110" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/fleetwood-town-leyton-orient/vJ9zGgZ9/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/port-vale-bolton/U72mDiJS/</t>
         </is>
       </c>
     </row>
@@ -10601,7 +10601,7 @@
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>Exeter</t>
+          <t>Shrewsbury</t>
         </is>
       </c>
       <c r="G111" t="n">
@@ -10609,63 +10609,63 @@
       </c>
       <c r="H111" t="inlineStr">
         <is>
-          <t>Northampton</t>
+          <t>Charlton</t>
         </is>
       </c>
       <c r="I111" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J111" t="n">
-        <v>1.73</v>
+        <v>2.67</v>
       </c>
       <c r="K111" t="inlineStr">
         <is>
-          <t>24/09/2023 03:13</t>
+          <t>23/09/2023 17:13</t>
         </is>
       </c>
       <c r="L111" t="n">
-        <v>2.13</v>
+        <v>3.08</v>
       </c>
       <c r="M111" t="inlineStr">
         <is>
-          <t>30/09/2023 15:51</t>
+          <t>30/09/2023 15:57</t>
         </is>
       </c>
       <c r="N111" t="n">
-        <v>3.48</v>
+        <v>3.15</v>
       </c>
       <c r="O111" t="inlineStr">
         <is>
-          <t>24/09/2023 03:13</t>
+          <t>23/09/2023 17:13</t>
         </is>
       </c>
       <c r="P111" t="n">
-        <v>3.53</v>
+        <v>3.43</v>
       </c>
       <c r="Q111" t="inlineStr">
         <is>
-          <t>30/09/2023 15:51</t>
+          <t>30/09/2023 15:18</t>
         </is>
       </c>
       <c r="R111" t="n">
-        <v>5.01</v>
+        <v>2.71</v>
       </c>
       <c r="S111" t="inlineStr">
         <is>
-          <t>24/09/2023 03:13</t>
+          <t>23/09/2023 17:13</t>
         </is>
       </c>
       <c r="T111" t="n">
-        <v>3.57</v>
+        <v>2.4</v>
       </c>
       <c r="U111" t="inlineStr">
         <is>
-          <t>30/09/2023 15:51</t>
+          <t>30/09/2023 15:57</t>
         </is>
       </c>
       <c r="V111" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/exeter-northampton/0SAWGZJ3/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/shrewsbury-charlton/vslJ7Vtj/</t>
         </is>
       </c>
     </row>
@@ -10693,71 +10693,71 @@
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>Derby</t>
+          <t>Stevenage</t>
         </is>
       </c>
       <c r="G112" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H112" t="inlineStr">
         <is>
-          <t>Cambridge Utd</t>
+          <t>Oxford Utd</t>
         </is>
       </c>
       <c r="I112" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J112" t="n">
-        <v>1.56</v>
+        <v>2.53</v>
       </c>
       <c r="K112" t="inlineStr">
         <is>
-          <t>23/09/2023 17:13</t>
+          <t>24/09/2023 03:13</t>
         </is>
       </c>
       <c r="L112" t="n">
-        <v>1.64</v>
+        <v>2.42</v>
       </c>
       <c r="M112" t="inlineStr">
         <is>
-          <t>30/09/2023 15:58</t>
+          <t>30/09/2023 15:51</t>
         </is>
       </c>
       <c r="N112" t="n">
-        <v>4.18</v>
+        <v>3.2</v>
       </c>
       <c r="O112" t="inlineStr">
         <is>
-          <t>23/09/2023 17:13</t>
+          <t>24/09/2023 03:13</t>
         </is>
       </c>
       <c r="P112" t="n">
-        <v>4.2</v>
+        <v>3.42</v>
       </c>
       <c r="Q112" t="inlineStr">
         <is>
-          <t>30/09/2023 15:58</t>
+          <t>30/09/2023 15:51</t>
         </is>
       </c>
       <c r="R112" t="n">
-        <v>5.3</v>
+        <v>2.83</v>
       </c>
       <c r="S112" t="inlineStr">
         <is>
-          <t>23/09/2023 17:13</t>
+          <t>24/09/2023 03:13</t>
         </is>
       </c>
       <c r="T112" t="n">
-        <v>5.29</v>
+        <v>3.06</v>
       </c>
       <c r="U112" t="inlineStr">
         <is>
-          <t>30/09/2023 15:58</t>
+          <t>30/09/2023 15:51</t>
         </is>
       </c>
       <c r="V112" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/derby-cambridge-utd/riGRHF4c/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/stevenage-oxford-utd/IXnN6kdd/</t>
         </is>
       </c>
     </row>
@@ -10785,22 +10785,22 @@
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>Barnsley</t>
+          <t>Wigan</t>
         </is>
       </c>
       <c r="G113" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H113" t="inlineStr">
         <is>
-          <t>Blackpool</t>
+          <t>Portsmouth</t>
         </is>
       </c>
       <c r="I113" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J113" t="n">
-        <v>2.18</v>
+        <v>3.14</v>
       </c>
       <c r="K113" t="inlineStr">
         <is>
@@ -10808,15 +10808,15 @@
         </is>
       </c>
       <c r="L113" t="n">
-        <v>2.51</v>
+        <v>3.11</v>
       </c>
       <c r="M113" t="inlineStr">
         <is>
-          <t>30/09/2023 15:50</t>
+          <t>30/09/2023 14:21</t>
         </is>
       </c>
       <c r="N113" t="n">
-        <v>3.31</v>
+        <v>3.21</v>
       </c>
       <c r="O113" t="inlineStr">
         <is>
@@ -10824,15 +10824,15 @@
         </is>
       </c>
       <c r="P113" t="n">
-        <v>3.6</v>
+        <v>3.59</v>
       </c>
       <c r="Q113" t="inlineStr">
         <is>
-          <t>30/09/2023 15:50</t>
+          <t>30/09/2023 15:38</t>
         </is>
       </c>
       <c r="R113" t="n">
-        <v>3.55</v>
+        <v>2.42</v>
       </c>
       <c r="S113" t="inlineStr">
         <is>
@@ -10840,16 +10840,16 @@
         </is>
       </c>
       <c r="T113" t="n">
-        <v>2.81</v>
+        <v>2.31</v>
       </c>
       <c r="U113" t="inlineStr">
         <is>
-          <t>30/09/2023 15:51</t>
+          <t>30/09/2023 14:21</t>
         </is>
       </c>
       <c r="V113" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/barnsley-blackpool/40HNIeki/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/wigan-portsmouth/KxR5VYYd/</t>
         </is>
       </c>
     </row>
@@ -10877,7 +10877,7 @@
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>Peterborough</t>
+          <t>Wycombe</t>
         </is>
       </c>
       <c r="G114" t="n">
@@ -10885,63 +10885,63 @@
       </c>
       <c r="H114" t="inlineStr">
         <is>
-          <t>Bristol Rovers</t>
+          <t>Carlisle</t>
         </is>
       </c>
       <c r="I114" t="n">
         <v>0</v>
       </c>
       <c r="J114" t="n">
-        <v>1.77</v>
+        <v>1.78</v>
       </c>
       <c r="K114" t="inlineStr">
         <is>
-          <t>23/09/2023 17:13</t>
+          <t>24/09/2023 03:13</t>
         </is>
       </c>
       <c r="L114" t="n">
-        <v>1.83</v>
+        <v>1.96</v>
       </c>
       <c r="M114" t="inlineStr">
         <is>
-          <t>30/09/2023 15:52</t>
+          <t>30/09/2023 15:51</t>
         </is>
       </c>
       <c r="N114" t="n">
-        <v>3.96</v>
+        <v>3.7</v>
       </c>
       <c r="O114" t="inlineStr">
         <is>
-          <t>23/09/2023 17:13</t>
+          <t>24/09/2023 03:13</t>
         </is>
       </c>
       <c r="P114" t="n">
-        <v>3.97</v>
+        <v>3.41</v>
       </c>
       <c r="Q114" t="inlineStr">
         <is>
-          <t>30/09/2023 15:52</t>
+          <t>30/09/2023 15:51</t>
         </is>
       </c>
       <c r="R114" t="n">
-        <v>4.05</v>
+        <v>4.31</v>
       </c>
       <c r="S114" t="inlineStr">
         <is>
-          <t>23/09/2023 17:13</t>
+          <t>24/09/2023 03:13</t>
         </is>
       </c>
       <c r="T114" t="n">
-        <v>4.23</v>
+        <v>4.31</v>
       </c>
       <c r="U114" t="inlineStr">
         <is>
-          <t>30/09/2023 15:52</t>
+          <t>30/09/2023 15:51</t>
         </is>
       </c>
       <c r="V114" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/peterborough-bristol-rovers/nqDrEX3M/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/wycombe-carlisle/YuV9Uhl3/</t>
         </is>
       </c>
     </row>
@@ -10969,22 +10969,22 @@
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>Cheltenham</t>
+          <t>Oxford Utd</t>
         </is>
       </c>
       <c r="G115" t="n">
+        <v>3</v>
+      </c>
+      <c r="H115" t="inlineStr">
+        <is>
+          <t>Shrewsbury</t>
+        </is>
+      </c>
+      <c r="I115" t="n">
         <v>0</v>
       </c>
-      <c r="H115" t="inlineStr">
-        <is>
-          <t>Fleetwood</t>
-        </is>
-      </c>
-      <c r="I115" t="n">
-        <v>2</v>
-      </c>
       <c r="J115" t="n">
-        <v>2.98</v>
+        <v>1.56</v>
       </c>
       <c r="K115" t="inlineStr">
         <is>
@@ -10992,15 +10992,15 @@
         </is>
       </c>
       <c r="L115" t="n">
-        <v>3.37</v>
+        <v>1.53</v>
       </c>
       <c r="M115" t="inlineStr">
         <is>
-          <t>03/10/2023 20:30</t>
+          <t>03/10/2023 20:33</t>
         </is>
       </c>
       <c r="N115" t="n">
-        <v>3.32</v>
+        <v>4.11</v>
       </c>
       <c r="O115" t="inlineStr">
         <is>
@@ -11008,15 +11008,15 @@
         </is>
       </c>
       <c r="P115" t="n">
-        <v>3.19</v>
+        <v>4.21</v>
       </c>
       <c r="Q115" t="inlineStr">
         <is>
-          <t>03/10/2023 20:08</t>
+          <t>03/10/2023 20:33</t>
         </is>
       </c>
       <c r="R115" t="n">
-        <v>2.36</v>
+        <v>6.08</v>
       </c>
       <c r="S115" t="inlineStr">
         <is>
@@ -11024,16 +11024,16 @@
         </is>
       </c>
       <c r="T115" t="n">
-        <v>2.36</v>
+        <v>6.92</v>
       </c>
       <c r="U115" t="inlineStr">
         <is>
-          <t>03/10/2023 20:30</t>
+          <t>03/10/2023 20:33</t>
         </is>
       </c>
       <c r="V115" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/cheltenham-fleetwood-town/hj15JSu2/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/oxford-utd-shrewsbury/2LrdtjmF/</t>
         </is>
       </c>
     </row>
@@ -11061,71 +11061,71 @@
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>Portsmouth</t>
+          <t>Northampton</t>
         </is>
       </c>
       <c r="G116" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H116" t="inlineStr">
         <is>
-          <t>Wycombe</t>
+          <t>Reading</t>
         </is>
       </c>
       <c r="I116" t="n">
         <v>1</v>
       </c>
       <c r="J116" t="n">
-        <v>1.78</v>
+        <v>2.41</v>
       </c>
       <c r="K116" t="inlineStr">
         <is>
-          <t>30/09/2023 17:13</t>
+          <t>30/09/2023 22:42</t>
         </is>
       </c>
       <c r="L116" t="n">
-        <v>1.8</v>
+        <v>2.43</v>
       </c>
       <c r="M116" t="inlineStr">
         <is>
-          <t>03/10/2023 19:21</t>
+          <t>03/10/2023 20:44</t>
         </is>
       </c>
       <c r="N116" t="n">
-        <v>3.78</v>
+        <v>3.49</v>
       </c>
       <c r="O116" t="inlineStr">
         <is>
-          <t>30/09/2023 17:13</t>
+          <t>30/09/2023 22:42</t>
         </is>
       </c>
       <c r="P116" t="n">
-        <v>3.72</v>
+        <v>3.54</v>
       </c>
       <c r="Q116" t="inlineStr">
         <is>
-          <t>03/10/2023 19:57</t>
+          <t>03/10/2023 20:44</t>
         </is>
       </c>
       <c r="R116" t="n">
-        <v>4.57</v>
+        <v>2.79</v>
       </c>
       <c r="S116" t="inlineStr">
         <is>
-          <t>30/09/2023 17:13</t>
+          <t>30/09/2023 22:42</t>
         </is>
       </c>
       <c r="T116" t="n">
-        <v>4.73</v>
+        <v>2.95</v>
       </c>
       <c r="U116" t="inlineStr">
         <is>
-          <t>03/10/2023 19:57</t>
+          <t>03/10/2023 20:44</t>
         </is>
       </c>
       <c r="V116" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/portsmouth-wycombe/GOn0uA2L/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/northampton-reading/KdgisWX8/</t>
         </is>
       </c>
     </row>
@@ -11153,22 +11153,22 @@
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>Oxford Utd</t>
+          <t>Cheltenham</t>
         </is>
       </c>
       <c r="G117" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H117" t="inlineStr">
         <is>
-          <t>Shrewsbury</t>
+          <t>Fleetwood</t>
         </is>
       </c>
       <c r="I117" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J117" t="n">
-        <v>1.56</v>
+        <v>2.98</v>
       </c>
       <c r="K117" t="inlineStr">
         <is>
@@ -11176,15 +11176,15 @@
         </is>
       </c>
       <c r="L117" t="n">
-        <v>1.53</v>
+        <v>3.37</v>
       </c>
       <c r="M117" t="inlineStr">
         <is>
-          <t>03/10/2023 20:33</t>
+          <t>03/10/2023 20:30</t>
         </is>
       </c>
       <c r="N117" t="n">
-        <v>4.11</v>
+        <v>3.32</v>
       </c>
       <c r="O117" t="inlineStr">
         <is>
@@ -11192,15 +11192,15 @@
         </is>
       </c>
       <c r="P117" t="n">
-        <v>4.21</v>
+        <v>3.19</v>
       </c>
       <c r="Q117" t="inlineStr">
         <is>
-          <t>03/10/2023 20:33</t>
+          <t>03/10/2023 20:08</t>
         </is>
       </c>
       <c r="R117" t="n">
-        <v>6.08</v>
+        <v>2.36</v>
       </c>
       <c r="S117" t="inlineStr">
         <is>
@@ -11208,16 +11208,16 @@
         </is>
       </c>
       <c r="T117" t="n">
-        <v>6.92</v>
+        <v>2.36</v>
       </c>
       <c r="U117" t="inlineStr">
         <is>
-          <t>03/10/2023 20:33</t>
+          <t>03/10/2023 20:30</t>
         </is>
       </c>
       <c r="V117" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/oxford-utd-shrewsbury/2LrdtjmF/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/cheltenham-fleetwood-town/hj15JSu2/</t>
         </is>
       </c>
     </row>
@@ -11245,71 +11245,71 @@
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>Carlisle</t>
+          <t>Portsmouth</t>
         </is>
       </c>
       <c r="G118" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H118" t="inlineStr">
         <is>
-          <t>Peterborough</t>
+          <t>Wycombe</t>
         </is>
       </c>
       <c r="I118" t="n">
         <v>1</v>
       </c>
       <c r="J118" t="n">
-        <v>3.49</v>
+        <v>1.78</v>
       </c>
       <c r="K118" t="inlineStr">
         <is>
-          <t>30/09/2023 22:42</t>
+          <t>30/09/2023 17:13</t>
         </is>
       </c>
       <c r="L118" t="n">
-        <v>3.66</v>
+        <v>1.8</v>
       </c>
       <c r="M118" t="inlineStr">
         <is>
-          <t>03/10/2023 20:44</t>
+          <t>03/10/2023 19:21</t>
         </is>
       </c>
       <c r="N118" t="n">
-        <v>3.52</v>
+        <v>3.78</v>
       </c>
       <c r="O118" t="inlineStr">
         <is>
-          <t>30/09/2023 22:42</t>
+          <t>30/09/2023 17:13</t>
         </is>
       </c>
       <c r="P118" t="n">
-        <v>3.62</v>
+        <v>3.72</v>
       </c>
       <c r="Q118" t="inlineStr">
         <is>
-          <t>03/10/2023 20:44</t>
+          <t>03/10/2023 19:57</t>
         </is>
       </c>
       <c r="R118" t="n">
-        <v>2.11</v>
+        <v>4.57</v>
       </c>
       <c r="S118" t="inlineStr">
         <is>
-          <t>30/09/2023 22:42</t>
+          <t>30/09/2023 17:13</t>
         </is>
       </c>
       <c r="T118" t="n">
-        <v>2.06</v>
+        <v>4.73</v>
       </c>
       <c r="U118" t="inlineStr">
         <is>
-          <t>03/10/2023 20:44</t>
+          <t>03/10/2023 19:57</t>
         </is>
       </c>
       <c r="V118" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/carlisle-peterborough/WzDdLlBk/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/portsmouth-wycombe/GOn0uA2L/</t>
         </is>
       </c>
     </row>
@@ -11337,22 +11337,22 @@
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>Northampton</t>
+          <t>Carlisle</t>
         </is>
       </c>
       <c r="G119" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H119" t="inlineStr">
         <is>
-          <t>Reading</t>
+          <t>Peterborough</t>
         </is>
       </c>
       <c r="I119" t="n">
         <v>1</v>
       </c>
       <c r="J119" t="n">
-        <v>2.41</v>
+        <v>3.49</v>
       </c>
       <c r="K119" t="inlineStr">
         <is>
@@ -11360,7 +11360,7 @@
         </is>
       </c>
       <c r="L119" t="n">
-        <v>2.43</v>
+        <v>3.66</v>
       </c>
       <c r="M119" t="inlineStr">
         <is>
@@ -11368,7 +11368,7 @@
         </is>
       </c>
       <c r="N119" t="n">
-        <v>3.49</v>
+        <v>3.52</v>
       </c>
       <c r="O119" t="inlineStr">
         <is>
@@ -11376,7 +11376,7 @@
         </is>
       </c>
       <c r="P119" t="n">
-        <v>3.54</v>
+        <v>3.62</v>
       </c>
       <c r="Q119" t="inlineStr">
         <is>
@@ -11384,7 +11384,7 @@
         </is>
       </c>
       <c r="R119" t="n">
-        <v>2.79</v>
+        <v>2.11</v>
       </c>
       <c r="S119" t="inlineStr">
         <is>
@@ -11392,7 +11392,7 @@
         </is>
       </c>
       <c r="T119" t="n">
-        <v>2.95</v>
+        <v>2.06</v>
       </c>
       <c r="U119" t="inlineStr">
         <is>
@@ -11401,7 +11401,7 @@
       </c>
       <c r="V119" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/northampton-reading/KdgisWX8/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/carlisle-peterborough/WzDdLlBk/</t>
         </is>
       </c>
     </row>
@@ -11429,71 +11429,71 @@
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>Burton</t>
+          <t>Charlton</t>
         </is>
       </c>
       <c r="G120" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H120" t="inlineStr">
         <is>
-          <t>Wigan</t>
+          <t>Exeter</t>
         </is>
       </c>
       <c r="I120" t="n">
         <v>1</v>
       </c>
       <c r="J120" t="n">
-        <v>2.98</v>
+        <v>2.17</v>
       </c>
       <c r="K120" t="inlineStr">
         <is>
-          <t>30/09/2023 22:42</t>
+          <t>30/09/2023 17:13</t>
         </is>
       </c>
       <c r="L120" t="n">
-        <v>2.62</v>
+        <v>1.87</v>
       </c>
       <c r="M120" t="inlineStr">
         <is>
-          <t>03/10/2023 20:31</t>
+          <t>03/10/2023 20:35</t>
         </is>
       </c>
       <c r="N120" t="n">
-        <v>3.44</v>
+        <v>3.49</v>
       </c>
       <c r="O120" t="inlineStr">
         <is>
-          <t>30/09/2023 22:42</t>
+          <t>30/09/2023 17:13</t>
         </is>
       </c>
       <c r="P120" t="n">
-        <v>3.28</v>
+        <v>3.83</v>
       </c>
       <c r="Q120" t="inlineStr">
         <is>
-          <t>03/10/2023 20:22</t>
+          <t>03/10/2023 20:35</t>
         </is>
       </c>
       <c r="R120" t="n">
-        <v>2.4</v>
+        <v>3.38</v>
       </c>
       <c r="S120" t="inlineStr">
         <is>
-          <t>30/09/2023 22:42</t>
+          <t>30/09/2023 17:13</t>
         </is>
       </c>
       <c r="T120" t="n">
-        <v>2.88</v>
+        <v>4.17</v>
       </c>
       <c r="U120" t="inlineStr">
         <is>
-          <t>03/10/2023 20:31</t>
+          <t>03/10/2023 20:35</t>
         </is>
       </c>
       <c r="V120" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/burton-wigan/2LMQQAmS/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/charlton-exeter/Ea21K8Qe/</t>
         </is>
       </c>
     </row>
@@ -11521,71 +11521,71 @@
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>Cambridge Utd</t>
+          <t>Burton</t>
         </is>
       </c>
       <c r="G121" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H121" t="inlineStr">
         <is>
-          <t>Barnsley</t>
+          <t>Wigan</t>
         </is>
       </c>
       <c r="I121" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J121" t="n">
-        <v>2.61</v>
+        <v>2.98</v>
       </c>
       <c r="K121" t="inlineStr">
         <is>
-          <t>30/09/2023 17:13</t>
+          <t>30/09/2023 22:42</t>
         </is>
       </c>
       <c r="L121" t="n">
-        <v>2.84</v>
+        <v>2.62</v>
       </c>
       <c r="M121" t="inlineStr">
         <is>
-          <t>03/10/2023 20:19</t>
+          <t>03/10/2023 20:31</t>
         </is>
       </c>
       <c r="N121" t="n">
-        <v>3.37</v>
+        <v>3.44</v>
       </c>
       <c r="O121" t="inlineStr">
         <is>
-          <t>30/09/2023 17:13</t>
+          <t>30/09/2023 22:42</t>
         </is>
       </c>
       <c r="P121" t="n">
-        <v>3.52</v>
+        <v>3.28</v>
       </c>
       <c r="Q121" t="inlineStr">
         <is>
-          <t>03/10/2023 20:19</t>
+          <t>03/10/2023 20:22</t>
         </is>
       </c>
       <c r="R121" t="n">
-        <v>2.64</v>
+        <v>2.4</v>
       </c>
       <c r="S121" t="inlineStr">
         <is>
-          <t>30/09/2023 17:13</t>
+          <t>30/09/2023 22:42</t>
         </is>
       </c>
       <c r="T121" t="n">
-        <v>2.52</v>
+        <v>2.88</v>
       </c>
       <c r="U121" t="inlineStr">
         <is>
-          <t>03/10/2023 20:19</t>
+          <t>03/10/2023 20:31</t>
         </is>
       </c>
       <c r="V121" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/cambridge-utd-barnsley/K09hMUeq/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/burton-wigan/2LMQQAmS/</t>
         </is>
       </c>
     </row>
@@ -11613,71 +11613,71 @@
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>Blackpool</t>
+          <t>Bristol Rovers</t>
         </is>
       </c>
       <c r="G122" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H122" t="inlineStr">
         <is>
-          <t>Derby</t>
+          <t>Port Vale</t>
         </is>
       </c>
       <c r="I122" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J122" t="n">
-        <v>2.26</v>
+        <v>2.06</v>
       </c>
       <c r="K122" t="inlineStr">
         <is>
-          <t>30/09/2023 22:42</t>
+          <t>30/09/2023 17:13</t>
         </is>
       </c>
       <c r="L122" t="n">
-        <v>2.57</v>
+        <v>2.08</v>
       </c>
       <c r="M122" t="inlineStr">
         <is>
-          <t>03/10/2023 20:26</t>
+          <t>03/10/2023 20:32</t>
         </is>
       </c>
       <c r="N122" t="n">
-        <v>3.5</v>
+        <v>3.47</v>
       </c>
       <c r="O122" t="inlineStr">
         <is>
-          <t>30/09/2023 22:42</t>
+          <t>30/09/2023 17:13</t>
         </is>
       </c>
       <c r="P122" t="n">
-        <v>3.24</v>
+        <v>3.54</v>
       </c>
       <c r="Q122" t="inlineStr">
         <is>
-          <t>03/10/2023 20:37</t>
+          <t>03/10/2023 20:32</t>
         </is>
       </c>
       <c r="R122" t="n">
-        <v>3</v>
+        <v>3.71</v>
       </c>
       <c r="S122" t="inlineStr">
         <is>
-          <t>30/09/2023 22:42</t>
+          <t>30/09/2023 17:13</t>
         </is>
       </c>
       <c r="T122" t="n">
-        <v>2.97</v>
+        <v>3.7</v>
       </c>
       <c r="U122" t="inlineStr">
         <is>
-          <t>03/10/2023 20:26</t>
+          <t>03/10/2023 20:32</t>
         </is>
       </c>
       <c r="V122" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/blackpool-derby/S2UDTC39/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/bristol-rovers-port-vale/OUNMRjYL/</t>
         </is>
       </c>
     </row>
@@ -11797,71 +11797,71 @@
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>Charlton</t>
+          <t>Blackpool</t>
         </is>
       </c>
       <c r="G124" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H124" t="inlineStr">
         <is>
-          <t>Exeter</t>
+          <t>Derby</t>
         </is>
       </c>
       <c r="I124" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J124" t="n">
-        <v>2.17</v>
+        <v>2.26</v>
       </c>
       <c r="K124" t="inlineStr">
         <is>
-          <t>30/09/2023 17:13</t>
+          <t>30/09/2023 22:42</t>
         </is>
       </c>
       <c r="L124" t="n">
-        <v>1.87</v>
+        <v>2.57</v>
       </c>
       <c r="M124" t="inlineStr">
         <is>
-          <t>03/10/2023 20:35</t>
+          <t>03/10/2023 20:26</t>
         </is>
       </c>
       <c r="N124" t="n">
-        <v>3.49</v>
+        <v>3.5</v>
       </c>
       <c r="O124" t="inlineStr">
         <is>
-          <t>30/09/2023 17:13</t>
+          <t>30/09/2023 22:42</t>
         </is>
       </c>
       <c r="P124" t="n">
-        <v>3.83</v>
+        <v>3.24</v>
       </c>
       <c r="Q124" t="inlineStr">
         <is>
-          <t>03/10/2023 20:35</t>
+          <t>03/10/2023 20:37</t>
         </is>
       </c>
       <c r="R124" t="n">
-        <v>3.38</v>
+        <v>3</v>
       </c>
       <c r="S124" t="inlineStr">
         <is>
-          <t>30/09/2023 17:13</t>
+          <t>30/09/2023 22:42</t>
         </is>
       </c>
       <c r="T124" t="n">
-        <v>4.17</v>
+        <v>2.97</v>
       </c>
       <c r="U124" t="inlineStr">
         <is>
-          <t>03/10/2023 20:35</t>
+          <t>03/10/2023 20:26</t>
         </is>
       </c>
       <c r="V124" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/charlton-exeter/Ea21K8Qe/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/blackpool-derby/S2UDTC39/</t>
         </is>
       </c>
     </row>
@@ -11889,22 +11889,22 @@
       </c>
       <c r="F125" t="inlineStr">
         <is>
-          <t>Bristol Rovers</t>
+          <t>Cambridge Utd</t>
         </is>
       </c>
       <c r="G125" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H125" t="inlineStr">
         <is>
-          <t>Port Vale</t>
+          <t>Barnsley</t>
         </is>
       </c>
       <c r="I125" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J125" t="n">
-        <v>2.06</v>
+        <v>2.61</v>
       </c>
       <c r="K125" t="inlineStr">
         <is>
@@ -11912,15 +11912,15 @@
         </is>
       </c>
       <c r="L125" t="n">
-        <v>2.08</v>
+        <v>2.84</v>
       </c>
       <c r="M125" t="inlineStr">
         <is>
-          <t>03/10/2023 20:32</t>
+          <t>03/10/2023 20:19</t>
         </is>
       </c>
       <c r="N125" t="n">
-        <v>3.47</v>
+        <v>3.37</v>
       </c>
       <c r="O125" t="inlineStr">
         <is>
@@ -11928,15 +11928,15 @@
         </is>
       </c>
       <c r="P125" t="n">
-        <v>3.54</v>
+        <v>3.52</v>
       </c>
       <c r="Q125" t="inlineStr">
         <is>
-          <t>03/10/2023 20:32</t>
+          <t>03/10/2023 20:19</t>
         </is>
       </c>
       <c r="R125" t="n">
-        <v>3.71</v>
+        <v>2.64</v>
       </c>
       <c r="S125" t="inlineStr">
         <is>
@@ -11944,16 +11944,16 @@
         </is>
       </c>
       <c r="T125" t="n">
-        <v>3.7</v>
+        <v>2.52</v>
       </c>
       <c r="U125" t="inlineStr">
         <is>
-          <t>03/10/2023 20:32</t>
+          <t>03/10/2023 20:19</t>
         </is>
       </c>
       <c r="V125" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/bristol-rovers-port-vale/OUNMRjYL/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/cambridge-utd-barnsley/K09hMUeq/</t>
         </is>
       </c>
     </row>
@@ -12073,22 +12073,22 @@
       </c>
       <c r="F127" t="inlineStr">
         <is>
-          <t>Stevenage</t>
+          <t>Peterborough</t>
         </is>
       </c>
       <c r="G127" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H127" t="inlineStr">
         <is>
-          <t>Wigan</t>
+          <t>Lincoln</t>
         </is>
       </c>
       <c r="I127" t="n">
         <v>0</v>
       </c>
       <c r="J127" t="n">
-        <v>1.78</v>
+        <v>1.76</v>
       </c>
       <c r="K127" t="inlineStr">
         <is>
@@ -12096,15 +12096,15 @@
         </is>
       </c>
       <c r="L127" t="n">
-        <v>1.82</v>
+        <v>1.61</v>
       </c>
       <c r="M127" t="inlineStr">
         <is>
-          <t>07/10/2023 15:49</t>
+          <t>07/10/2023 15:52</t>
         </is>
       </c>
       <c r="N127" t="n">
-        <v>3.81</v>
+        <v>3.75</v>
       </c>
       <c r="O127" t="inlineStr">
         <is>
@@ -12112,15 +12112,15 @@
         </is>
       </c>
       <c r="P127" t="n">
-        <v>3.61</v>
+        <v>4.07</v>
       </c>
       <c r="Q127" t="inlineStr">
         <is>
-          <t>07/10/2023 15:49</t>
+          <t>07/10/2023 16:00</t>
         </is>
       </c>
       <c r="R127" t="n">
-        <v>4.15</v>
+        <v>4.71</v>
       </c>
       <c r="S127" t="inlineStr">
         <is>
@@ -12128,16 +12128,16 @@
         </is>
       </c>
       <c r="T127" t="n">
-        <v>4.8</v>
+        <v>5.88</v>
       </c>
       <c r="U127" t="inlineStr">
         <is>
-          <t>07/10/2023 15:49</t>
+          <t>07/10/2023 16:00</t>
         </is>
       </c>
       <c r="V127" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/stevenage-wigan/6R47ZvWa/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/peterborough-lincoln-city/YyDfxsns/</t>
         </is>
       </c>
     </row>
@@ -12165,22 +12165,22 @@
       </c>
       <c r="F128" t="inlineStr">
         <is>
-          <t>Portsmouth</t>
+          <t>Stevenage</t>
         </is>
       </c>
       <c r="G128" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H128" t="inlineStr">
         <is>
-          <t>Port Vale</t>
+          <t>Wigan</t>
         </is>
       </c>
       <c r="I128" t="n">
         <v>0</v>
       </c>
       <c r="J128" t="n">
-        <v>1.66</v>
+        <v>1.78</v>
       </c>
       <c r="K128" t="inlineStr">
         <is>
@@ -12188,15 +12188,15 @@
         </is>
       </c>
       <c r="L128" t="n">
-        <v>1.6</v>
+        <v>1.82</v>
       </c>
       <c r="M128" t="inlineStr">
         <is>
-          <t>07/10/2023 15:57</t>
+          <t>07/10/2023 15:49</t>
         </is>
       </c>
       <c r="N128" t="n">
-        <v>3.95</v>
+        <v>3.81</v>
       </c>
       <c r="O128" t="inlineStr">
         <is>
@@ -12204,15 +12204,15 @@
         </is>
       </c>
       <c r="P128" t="n">
-        <v>4.37</v>
+        <v>3.61</v>
       </c>
       <c r="Q128" t="inlineStr">
         <is>
-          <t>07/10/2023 15:57</t>
+          <t>07/10/2023 15:49</t>
         </is>
       </c>
       <c r="R128" t="n">
-        <v>5.22</v>
+        <v>4.15</v>
       </c>
       <c r="S128" t="inlineStr">
         <is>
@@ -12220,16 +12220,16 @@
         </is>
       </c>
       <c r="T128" t="n">
-        <v>5.52</v>
+        <v>4.8</v>
       </c>
       <c r="U128" t="inlineStr">
         <is>
-          <t>07/10/2023 15:57</t>
+          <t>07/10/2023 15:49</t>
         </is>
       </c>
       <c r="V128" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/portsmouth-port-vale/CSBby11m/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/stevenage-wigan/6R47ZvWa/</t>
         </is>
       </c>
     </row>
@@ -12257,22 +12257,22 @@
       </c>
       <c r="F129" t="inlineStr">
         <is>
-          <t>Leyton Orient</t>
+          <t>Shrewsbury</t>
         </is>
       </c>
       <c r="G129" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H129" t="inlineStr">
         <is>
-          <t>Reading</t>
+          <t>Northampton</t>
         </is>
       </c>
       <c r="I129" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J129" t="n">
-        <v>2.14</v>
+        <v>2.41</v>
       </c>
       <c r="K129" t="inlineStr">
         <is>
@@ -12280,15 +12280,15 @@
         </is>
       </c>
       <c r="L129" t="n">
-        <v>2.4</v>
+        <v>3.03</v>
       </c>
       <c r="M129" t="inlineStr">
         <is>
-          <t>07/10/2023 15:57</t>
+          <t>07/10/2023 15:58</t>
         </is>
       </c>
       <c r="N129" t="n">
-        <v>3.35</v>
+        <v>3.33</v>
       </c>
       <c r="O129" t="inlineStr">
         <is>
@@ -12296,15 +12296,15 @@
         </is>
       </c>
       <c r="P129" t="n">
-        <v>3.35</v>
+        <v>3.19</v>
       </c>
       <c r="Q129" t="inlineStr">
         <is>
-          <t>07/10/2023 15:52</t>
+          <t>07/10/2023 15:58</t>
         </is>
       </c>
       <c r="R129" t="n">
-        <v>3.39</v>
+        <v>2.9</v>
       </c>
       <c r="S129" t="inlineStr">
         <is>
@@ -12312,16 +12312,16 @@
         </is>
       </c>
       <c r="T129" t="n">
-        <v>3.14</v>
+        <v>2.57</v>
       </c>
       <c r="U129" t="inlineStr">
         <is>
-          <t>07/10/2023 15:52</t>
+          <t>07/10/2023 15:58</t>
         </is>
       </c>
       <c r="V129" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/leyton-orient-reading/SxoNfk28/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/shrewsbury-northampton/fi13zLGg/</t>
         </is>
       </c>
     </row>
@@ -12349,22 +12349,22 @@
       </c>
       <c r="F130" t="inlineStr">
         <is>
-          <t>Fleetwood</t>
+          <t>Portsmouth</t>
         </is>
       </c>
       <c r="G130" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H130" t="inlineStr">
         <is>
-          <t>Wycombe</t>
+          <t>Port Vale</t>
         </is>
       </c>
       <c r="I130" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J130" t="n">
-        <v>2.43</v>
+        <v>1.66</v>
       </c>
       <c r="K130" t="inlineStr">
         <is>
@@ -12372,15 +12372,15 @@
         </is>
       </c>
       <c r="L130" t="n">
-        <v>2.29</v>
+        <v>1.6</v>
       </c>
       <c r="M130" t="inlineStr">
         <is>
-          <t>07/10/2023 15:50</t>
+          <t>07/10/2023 15:57</t>
         </is>
       </c>
       <c r="N130" t="n">
-        <v>3.27</v>
+        <v>3.95</v>
       </c>
       <c r="O130" t="inlineStr">
         <is>
@@ -12388,15 +12388,15 @@
         </is>
       </c>
       <c r="P130" t="n">
-        <v>3.37</v>
+        <v>4.37</v>
       </c>
       <c r="Q130" t="inlineStr">
         <is>
-          <t>07/10/2023 15:46</t>
+          <t>07/10/2023 15:57</t>
         </is>
       </c>
       <c r="R130" t="n">
-        <v>3.07</v>
+        <v>5.22</v>
       </c>
       <c r="S130" t="inlineStr">
         <is>
@@ -12404,16 +12404,16 @@
         </is>
       </c>
       <c r="T130" t="n">
-        <v>3.34</v>
+        <v>5.52</v>
       </c>
       <c r="U130" t="inlineStr">
         <is>
-          <t>07/10/2023 15:50</t>
+          <t>07/10/2023 15:57</t>
         </is>
       </c>
       <c r="V130" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/fleetwood-town-wycombe/QX6vW5P7/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/portsmouth-port-vale/CSBby11m/</t>
         </is>
       </c>
     </row>
@@ -12441,22 +12441,22 @@
       </c>
       <c r="F131" t="inlineStr">
         <is>
-          <t>Shrewsbury</t>
+          <t>Leyton Orient</t>
         </is>
       </c>
       <c r="G131" t="n">
+        <v>2</v>
+      </c>
+      <c r="H131" t="inlineStr">
+        <is>
+          <t>Reading</t>
+        </is>
+      </c>
+      <c r="I131" t="n">
         <v>1</v>
       </c>
-      <c r="H131" t="inlineStr">
-        <is>
-          <t>Northampton</t>
-        </is>
-      </c>
-      <c r="I131" t="n">
-        <v>0</v>
-      </c>
       <c r="J131" t="n">
-        <v>2.41</v>
+        <v>2.14</v>
       </c>
       <c r="K131" t="inlineStr">
         <is>
@@ -12464,15 +12464,15 @@
         </is>
       </c>
       <c r="L131" t="n">
-        <v>3.03</v>
+        <v>2.4</v>
       </c>
       <c r="M131" t="inlineStr">
         <is>
-          <t>07/10/2023 15:58</t>
+          <t>07/10/2023 15:57</t>
         </is>
       </c>
       <c r="N131" t="n">
-        <v>3.33</v>
+        <v>3.35</v>
       </c>
       <c r="O131" t="inlineStr">
         <is>
@@ -12480,15 +12480,15 @@
         </is>
       </c>
       <c r="P131" t="n">
-        <v>3.19</v>
+        <v>3.35</v>
       </c>
       <c r="Q131" t="inlineStr">
         <is>
-          <t>07/10/2023 15:58</t>
+          <t>07/10/2023 15:52</t>
         </is>
       </c>
       <c r="R131" t="n">
-        <v>2.9</v>
+        <v>3.39</v>
       </c>
       <c r="S131" t="inlineStr">
         <is>
@@ -12496,16 +12496,16 @@
         </is>
       </c>
       <c r="T131" t="n">
-        <v>2.57</v>
+        <v>3.14</v>
       </c>
       <c r="U131" t="inlineStr">
         <is>
-          <t>07/10/2023 15:58</t>
+          <t>07/10/2023 15:52</t>
         </is>
       </c>
       <c r="V131" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/shrewsbury-northampton/fi13zLGg/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/leyton-orient-reading/SxoNfk28/</t>
         </is>
       </c>
     </row>
@@ -12533,7 +12533,7 @@
       </c>
       <c r="F132" t="inlineStr">
         <is>
-          <t>Cheltenham</t>
+          <t>Fleetwood</t>
         </is>
       </c>
       <c r="G132" t="n">
@@ -12541,14 +12541,14 @@
       </c>
       <c r="H132" t="inlineStr">
         <is>
-          <t>Derby</t>
+          <t>Wycombe</t>
         </is>
       </c>
       <c r="I132" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J132" t="n">
-        <v>4.29</v>
+        <v>2.43</v>
       </c>
       <c r="K132" t="inlineStr">
         <is>
@@ -12556,15 +12556,15 @@
         </is>
       </c>
       <c r="L132" t="n">
-        <v>6.41</v>
+        <v>2.29</v>
       </c>
       <c r="M132" t="inlineStr">
         <is>
-          <t>07/10/2023 15:39</t>
+          <t>07/10/2023 15:50</t>
         </is>
       </c>
       <c r="N132" t="n">
-        <v>3.7</v>
+        <v>3.27</v>
       </c>
       <c r="O132" t="inlineStr">
         <is>
@@ -12572,15 +12572,15 @@
         </is>
       </c>
       <c r="P132" t="n">
-        <v>4.02</v>
+        <v>3.37</v>
       </c>
       <c r="Q132" t="inlineStr">
         <is>
-          <t>07/10/2023 15:39</t>
+          <t>07/10/2023 15:46</t>
         </is>
       </c>
       <c r="R132" t="n">
-        <v>1.78</v>
+        <v>3.07</v>
       </c>
       <c r="S132" t="inlineStr">
         <is>
@@ -12588,16 +12588,16 @@
         </is>
       </c>
       <c r="T132" t="n">
-        <v>1.58</v>
+        <v>3.34</v>
       </c>
       <c r="U132" t="inlineStr">
         <is>
-          <t>07/10/2023 15:39</t>
+          <t>07/10/2023 15:50</t>
         </is>
       </c>
       <c r="V132" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/cheltenham-derby/I73WXRfe/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/fleetwood-town-wycombe/QX6vW5P7/</t>
         </is>
       </c>
     </row>
@@ -12625,22 +12625,22 @@
       </c>
       <c r="F133" t="inlineStr">
         <is>
-          <t>Charlton</t>
+          <t>Exeter</t>
         </is>
       </c>
       <c r="G133" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H133" t="inlineStr">
         <is>
-          <t>Blackpool</t>
+          <t>Barnsley</t>
         </is>
       </c>
       <c r="I133" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J133" t="n">
-        <v>2.5</v>
+        <v>2.26</v>
       </c>
       <c r="K133" t="inlineStr">
         <is>
@@ -12648,15 +12648,15 @@
         </is>
       </c>
       <c r="L133" t="n">
-        <v>2.36</v>
+        <v>2.93</v>
       </c>
       <c r="M133" t="inlineStr">
         <is>
-          <t>07/10/2023 15:53</t>
+          <t>07/10/2023 15:52</t>
         </is>
       </c>
       <c r="N133" t="n">
-        <v>3.32</v>
+        <v>3.38</v>
       </c>
       <c r="O133" t="inlineStr">
         <is>
@@ -12664,15 +12664,15 @@
         </is>
       </c>
       <c r="P133" t="n">
-        <v>3.41</v>
+        <v>3.46</v>
       </c>
       <c r="Q133" t="inlineStr">
         <is>
-          <t>07/10/2023 15:51</t>
+          <t>07/10/2023 15:52</t>
         </is>
       </c>
       <c r="R133" t="n">
-        <v>2.79</v>
+        <v>3.11</v>
       </c>
       <c r="S133" t="inlineStr">
         <is>
@@ -12680,16 +12680,16 @@
         </is>
       </c>
       <c r="T133" t="n">
-        <v>3.15</v>
+        <v>2.48</v>
       </c>
       <c r="U133" t="inlineStr">
         <is>
-          <t>07/10/2023 15:53</t>
+          <t>07/10/2023 15:52</t>
         </is>
       </c>
       <c r="V133" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/charlton-blackpool/vH4SY7uk/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/exeter-barnsley/CU2zXoA1/</t>
         </is>
       </c>
     </row>
@@ -12717,7 +12717,7 @@
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>Bolton</t>
+          <t>Cheltenham</t>
         </is>
       </c>
       <c r="G134" t="n">
@@ -12725,14 +12725,14 @@
       </c>
       <c r="H134" t="inlineStr">
         <is>
-          <t>Carlisle</t>
+          <t>Derby</t>
         </is>
       </c>
       <c r="I134" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J134" t="n">
-        <v>1.6</v>
+        <v>4.29</v>
       </c>
       <c r="K134" t="inlineStr">
         <is>
@@ -12740,15 +12740,15 @@
         </is>
       </c>
       <c r="L134" t="n">
-        <v>1.55</v>
+        <v>6.41</v>
       </c>
       <c r="M134" t="inlineStr">
         <is>
-          <t>07/10/2023 16:00</t>
+          <t>07/10/2023 15:39</t>
         </is>
       </c>
       <c r="N134" t="n">
-        <v>4.06</v>
+        <v>3.7</v>
       </c>
       <c r="O134" t="inlineStr">
         <is>
@@ -12756,15 +12756,15 @@
         </is>
       </c>
       <c r="P134" t="n">
-        <v>4.29</v>
+        <v>4.02</v>
       </c>
       <c r="Q134" t="inlineStr">
         <is>
-          <t>07/10/2023 16:00</t>
+          <t>07/10/2023 15:39</t>
         </is>
       </c>
       <c r="R134" t="n">
-        <v>5.69</v>
+        <v>1.78</v>
       </c>
       <c r="S134" t="inlineStr">
         <is>
@@ -12772,16 +12772,16 @@
         </is>
       </c>
       <c r="T134" t="n">
-        <v>6.25</v>
+        <v>1.58</v>
       </c>
       <c r="U134" t="inlineStr">
         <is>
-          <t>07/10/2023 16:00</t>
+          <t>07/10/2023 15:39</t>
         </is>
       </c>
       <c r="V134" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/bolton-carlisle/Aon4vUHR/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/cheltenham-derby/I73WXRfe/</t>
         </is>
       </c>
     </row>
@@ -12809,22 +12809,22 @@
       </c>
       <c r="F135" t="inlineStr">
         <is>
-          <t>Exeter</t>
+          <t>Charlton</t>
         </is>
       </c>
       <c r="G135" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H135" t="inlineStr">
         <is>
-          <t>Barnsley</t>
+          <t>Blackpool</t>
         </is>
       </c>
       <c r="I135" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J135" t="n">
-        <v>2.26</v>
+        <v>2.5</v>
       </c>
       <c r="K135" t="inlineStr">
         <is>
@@ -12832,15 +12832,15 @@
         </is>
       </c>
       <c r="L135" t="n">
-        <v>2.93</v>
+        <v>2.36</v>
       </c>
       <c r="M135" t="inlineStr">
         <is>
-          <t>07/10/2023 15:52</t>
+          <t>07/10/2023 15:53</t>
         </is>
       </c>
       <c r="N135" t="n">
-        <v>3.38</v>
+        <v>3.32</v>
       </c>
       <c r="O135" t="inlineStr">
         <is>
@@ -12848,15 +12848,15 @@
         </is>
       </c>
       <c r="P135" t="n">
-        <v>3.46</v>
+        <v>3.41</v>
       </c>
       <c r="Q135" t="inlineStr">
         <is>
-          <t>07/10/2023 15:52</t>
+          <t>07/10/2023 15:51</t>
         </is>
       </c>
       <c r="R135" t="n">
-        <v>3.11</v>
+        <v>2.79</v>
       </c>
       <c r="S135" t="inlineStr">
         <is>
@@ -12864,16 +12864,16 @@
         </is>
       </c>
       <c r="T135" t="n">
-        <v>2.48</v>
+        <v>3.15</v>
       </c>
       <c r="U135" t="inlineStr">
         <is>
-          <t>07/10/2023 15:52</t>
+          <t>07/10/2023 15:53</t>
         </is>
       </c>
       <c r="V135" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/exeter-barnsley/CU2zXoA1/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/charlton-blackpool/vH4SY7uk/</t>
         </is>
       </c>
     </row>
@@ -12901,22 +12901,22 @@
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>Peterborough</t>
+          <t>Bolton</t>
         </is>
       </c>
       <c r="G136" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H136" t="inlineStr">
         <is>
-          <t>Lincoln</t>
+          <t>Carlisle</t>
         </is>
       </c>
       <c r="I136" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J136" t="n">
-        <v>1.76</v>
+        <v>1.6</v>
       </c>
       <c r="K136" t="inlineStr">
         <is>
@@ -12924,15 +12924,15 @@
         </is>
       </c>
       <c r="L136" t="n">
-        <v>1.61</v>
+        <v>1.55</v>
       </c>
       <c r="M136" t="inlineStr">
         <is>
-          <t>07/10/2023 15:52</t>
+          <t>07/10/2023 16:00</t>
         </is>
       </c>
       <c r="N136" t="n">
-        <v>3.75</v>
+        <v>4.06</v>
       </c>
       <c r="O136" t="inlineStr">
         <is>
@@ -12940,7 +12940,7 @@
         </is>
       </c>
       <c r="P136" t="n">
-        <v>4.07</v>
+        <v>4.29</v>
       </c>
       <c r="Q136" t="inlineStr">
         <is>
@@ -12948,7 +12948,7 @@
         </is>
       </c>
       <c r="R136" t="n">
-        <v>4.71</v>
+        <v>5.69</v>
       </c>
       <c r="S136" t="inlineStr">
         <is>
@@ -12956,7 +12956,7 @@
         </is>
       </c>
       <c r="T136" t="n">
-        <v>5.88</v>
+        <v>6.25</v>
       </c>
       <c r="U136" t="inlineStr">
         <is>
@@ -12965,7 +12965,7 @@
       </c>
       <c r="V136" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/peterborough-lincoln-city/YyDfxsns/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/bolton-carlisle/Aon4vUHR/</t>
         </is>
       </c>
     </row>
@@ -13453,7 +13453,7 @@
       </c>
       <c r="F142" t="inlineStr">
         <is>
-          <t>Leyton Orient</t>
+          <t>Oxford Utd</t>
         </is>
       </c>
       <c r="G142" t="n">
@@ -13461,14 +13461,14 @@
       </c>
       <c r="H142" t="inlineStr">
         <is>
-          <t>Barnsley</t>
+          <t>Blackpool</t>
         </is>
       </c>
       <c r="I142" t="n">
         <v>1</v>
       </c>
       <c r="J142" t="n">
-        <v>2.8</v>
+        <v>1.89</v>
       </c>
       <c r="K142" t="inlineStr">
         <is>
@@ -13476,15 +13476,15 @@
         </is>
       </c>
       <c r="L142" t="n">
-        <v>2.67</v>
+        <v>2.03</v>
       </c>
       <c r="M142" t="inlineStr">
         <is>
-          <t>21/10/2023 15:46</t>
+          <t>21/10/2023 15:56</t>
         </is>
       </c>
       <c r="N142" t="n">
-        <v>3.38</v>
+        <v>3.64</v>
       </c>
       <c r="O142" t="inlineStr">
         <is>
@@ -13492,15 +13492,15 @@
         </is>
       </c>
       <c r="P142" t="n">
-        <v>3.35</v>
+        <v>3.53</v>
       </c>
       <c r="Q142" t="inlineStr">
         <is>
-          <t>21/10/2023 14:59</t>
+          <t>21/10/2023 15:56</t>
         </is>
       </c>
       <c r="R142" t="n">
-        <v>2.46</v>
+        <v>4.12</v>
       </c>
       <c r="S142" t="inlineStr">
         <is>
@@ -13508,16 +13508,16 @@
         </is>
       </c>
       <c r="T142" t="n">
-        <v>2.78</v>
+        <v>3.85</v>
       </c>
       <c r="U142" t="inlineStr">
         <is>
-          <t>21/10/2023 15:46</t>
+          <t>21/10/2023 15:56</t>
         </is>
       </c>
       <c r="V142" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/leyton-orient-barnsley/GvgSayp5/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/oxford-utd-blackpool/fViWbeaB/</t>
         </is>
       </c>
     </row>
@@ -13545,22 +13545,22 @@
       </c>
       <c r="F143" t="inlineStr">
         <is>
-          <t>Stevenage</t>
+          <t>Leyton Orient</t>
         </is>
       </c>
       <c r="G143" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H143" t="inlineStr">
         <is>
-          <t>Port Vale</t>
+          <t>Barnsley</t>
         </is>
       </c>
       <c r="I143" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J143" t="n">
-        <v>1.79</v>
+        <v>2.8</v>
       </c>
       <c r="K143" t="inlineStr">
         <is>
@@ -13568,15 +13568,15 @@
         </is>
       </c>
       <c r="L143" t="n">
-        <v>1.97</v>
+        <v>2.67</v>
       </c>
       <c r="M143" t="inlineStr">
         <is>
-          <t>21/10/2023 15:51</t>
+          <t>21/10/2023 15:46</t>
         </is>
       </c>
       <c r="N143" t="n">
-        <v>3.69</v>
+        <v>3.38</v>
       </c>
       <c r="O143" t="inlineStr">
         <is>
@@ -13584,15 +13584,15 @@
         </is>
       </c>
       <c r="P143" t="n">
-        <v>3.5</v>
+        <v>3.35</v>
       </c>
       <c r="Q143" t="inlineStr">
         <is>
-          <t>21/10/2023 15:52</t>
+          <t>21/10/2023 14:59</t>
         </is>
       </c>
       <c r="R143" t="n">
-        <v>4.65</v>
+        <v>2.46</v>
       </c>
       <c r="S143" t="inlineStr">
         <is>
@@ -13600,16 +13600,16 @@
         </is>
       </c>
       <c r="T143" t="n">
-        <v>4.15</v>
+        <v>2.78</v>
       </c>
       <c r="U143" t="inlineStr">
         <is>
-          <t>21/10/2023 15:51</t>
+          <t>21/10/2023 15:46</t>
         </is>
       </c>
       <c r="V143" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/stevenage-port-vale/MuxBiDio/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/leyton-orient-barnsley/GvgSayp5/</t>
         </is>
       </c>
     </row>
@@ -13821,22 +13821,22 @@
       </c>
       <c r="F146" t="inlineStr">
         <is>
-          <t>Oxford Utd</t>
+          <t>Stevenage</t>
         </is>
       </c>
       <c r="G146" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H146" t="inlineStr">
         <is>
-          <t>Blackpool</t>
+          <t>Port Vale</t>
         </is>
       </c>
       <c r="I146" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J146" t="n">
-        <v>1.89</v>
+        <v>1.79</v>
       </c>
       <c r="K146" t="inlineStr">
         <is>
@@ -13844,15 +13844,15 @@
         </is>
       </c>
       <c r="L146" t="n">
-        <v>2.03</v>
+        <v>1.97</v>
       </c>
       <c r="M146" t="inlineStr">
         <is>
-          <t>21/10/2023 15:56</t>
+          <t>21/10/2023 15:51</t>
         </is>
       </c>
       <c r="N146" t="n">
-        <v>3.64</v>
+        <v>3.69</v>
       </c>
       <c r="O146" t="inlineStr">
         <is>
@@ -13860,15 +13860,15 @@
         </is>
       </c>
       <c r="P146" t="n">
-        <v>3.53</v>
+        <v>3.5</v>
       </c>
       <c r="Q146" t="inlineStr">
         <is>
-          <t>21/10/2023 15:56</t>
+          <t>21/10/2023 15:52</t>
         </is>
       </c>
       <c r="R146" t="n">
-        <v>4.12</v>
+        <v>4.65</v>
       </c>
       <c r="S146" t="inlineStr">
         <is>
@@ -13876,16 +13876,16 @@
         </is>
       </c>
       <c r="T146" t="n">
-        <v>3.85</v>
+        <v>4.15</v>
       </c>
       <c r="U146" t="inlineStr">
         <is>
-          <t>21/10/2023 15:56</t>
+          <t>21/10/2023 15:51</t>
         </is>
       </c>
       <c r="V146" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/oxford-utd-blackpool/fViWbeaB/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/stevenage-port-vale/MuxBiDio/</t>
         </is>
       </c>
     </row>
@@ -15109,22 +15109,22 @@
       </c>
       <c r="F160" t="inlineStr">
         <is>
-          <t>Cambridge Utd</t>
+          <t>Carlisle</t>
         </is>
       </c>
       <c r="G160" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H160" t="inlineStr">
         <is>
-          <t>Portsmouth</t>
+          <t>Burton</t>
         </is>
       </c>
       <c r="I160" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J160" t="n">
-        <v>3.92</v>
+        <v>2.1</v>
       </c>
       <c r="K160" t="inlineStr">
         <is>
@@ -15132,15 +15132,15 @@
         </is>
       </c>
       <c r="L160" t="n">
-        <v>4.29</v>
+        <v>2.46</v>
       </c>
       <c r="M160" t="inlineStr">
         <is>
-          <t>24/10/2023 20:29</t>
+          <t>24/10/2023 20:41</t>
         </is>
       </c>
       <c r="N160" t="n">
-        <v>3.67</v>
+        <v>3.29</v>
       </c>
       <c r="O160" t="inlineStr">
         <is>
@@ -15148,15 +15148,15 @@
         </is>
       </c>
       <c r="P160" t="n">
-        <v>3.65</v>
+        <v>3.3</v>
       </c>
       <c r="Q160" t="inlineStr">
         <is>
-          <t>24/10/2023 20:29</t>
+          <t>24/10/2023 20:41</t>
         </is>
       </c>
       <c r="R160" t="n">
-        <v>1.87</v>
+        <v>3.57</v>
       </c>
       <c r="S160" t="inlineStr">
         <is>
@@ -15164,16 +15164,16 @@
         </is>
       </c>
       <c r="T160" t="n">
-        <v>1.89</v>
+        <v>3.09</v>
       </c>
       <c r="U160" t="inlineStr">
         <is>
-          <t>24/10/2023 20:04</t>
+          <t>24/10/2023 20:41</t>
         </is>
       </c>
       <c r="V160" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/cambridge-utd-portsmouth/YyubDfE4/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/carlisle-burton/Sbv2CETA/</t>
         </is>
       </c>
     </row>
@@ -15201,22 +15201,22 @@
       </c>
       <c r="F161" t="inlineStr">
         <is>
-          <t>Bristol Rovers</t>
+          <t>Cambridge Utd</t>
         </is>
       </c>
       <c r="G161" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H161" t="inlineStr">
         <is>
-          <t>Stevenage</t>
+          <t>Portsmouth</t>
         </is>
       </c>
       <c r="I161" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J161" t="n">
-        <v>2.63</v>
+        <v>3.92</v>
       </c>
       <c r="K161" t="inlineStr">
         <is>
@@ -15224,15 +15224,15 @@
         </is>
       </c>
       <c r="L161" t="n">
-        <v>2.42</v>
+        <v>4.29</v>
       </c>
       <c r="M161" t="inlineStr">
         <is>
-          <t>24/10/2023 20:41</t>
+          <t>24/10/2023 20:29</t>
         </is>
       </c>
       <c r="N161" t="n">
-        <v>3.29</v>
+        <v>3.67</v>
       </c>
       <c r="O161" t="inlineStr">
         <is>
@@ -15240,15 +15240,15 @@
         </is>
       </c>
       <c r="P161" t="n">
-        <v>3.39</v>
+        <v>3.65</v>
       </c>
       <c r="Q161" t="inlineStr">
         <is>
-          <t>24/10/2023 20:41</t>
+          <t>24/10/2023 20:29</t>
         </is>
       </c>
       <c r="R161" t="n">
-        <v>2.79</v>
+        <v>1.87</v>
       </c>
       <c r="S161" t="inlineStr">
         <is>
@@ -15256,16 +15256,16 @@
         </is>
       </c>
       <c r="T161" t="n">
-        <v>3.07</v>
+        <v>1.89</v>
       </c>
       <c r="U161" t="inlineStr">
         <is>
-          <t>24/10/2023 20:41</t>
+          <t>24/10/2023 20:04</t>
         </is>
       </c>
       <c r="V161" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/bristol-rovers-stevenage/fotfEzab/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/cambridge-utd-portsmouth/YyubDfE4/</t>
         </is>
       </c>
     </row>
@@ -15293,22 +15293,22 @@
       </c>
       <c r="F162" t="inlineStr">
         <is>
-          <t>Blackpool</t>
+          <t>Bristol Rovers</t>
         </is>
       </c>
       <c r="G162" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H162" t="inlineStr">
         <is>
-          <t>Cheltenham</t>
+          <t>Stevenage</t>
         </is>
       </c>
       <c r="I162" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J162" t="n">
-        <v>1.41</v>
+        <v>2.63</v>
       </c>
       <c r="K162" t="inlineStr">
         <is>
@@ -15316,15 +15316,15 @@
         </is>
       </c>
       <c r="L162" t="n">
-        <v>1.38</v>
+        <v>2.42</v>
       </c>
       <c r="M162" t="inlineStr">
         <is>
-          <t>24/10/2023 20:36</t>
+          <t>24/10/2023 20:41</t>
         </is>
       </c>
       <c r="N162" t="n">
-        <v>4.5</v>
+        <v>3.29</v>
       </c>
       <c r="O162" t="inlineStr">
         <is>
@@ -15332,7 +15332,7 @@
         </is>
       </c>
       <c r="P162" t="n">
-        <v>4.82</v>
+        <v>3.39</v>
       </c>
       <c r="Q162" t="inlineStr">
         <is>
@@ -15340,7 +15340,7 @@
         </is>
       </c>
       <c r="R162" t="n">
-        <v>7.23</v>
+        <v>2.79</v>
       </c>
       <c r="S162" t="inlineStr">
         <is>
@@ -15348,7 +15348,7 @@
         </is>
       </c>
       <c r="T162" t="n">
-        <v>9.26</v>
+        <v>3.07</v>
       </c>
       <c r="U162" t="inlineStr">
         <is>
@@ -15357,7 +15357,7 @@
       </c>
       <c r="V162" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/blackpool-cheltenham/EZOdFGqh/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/bristol-rovers-stevenage/fotfEzab/</t>
         </is>
       </c>
     </row>
@@ -15385,7 +15385,7 @@
       </c>
       <c r="F163" t="inlineStr">
         <is>
-          <t>Barnsley</t>
+          <t>Blackpool</t>
         </is>
       </c>
       <c r="G163" t="n">
@@ -15393,14 +15393,14 @@
       </c>
       <c r="H163" t="inlineStr">
         <is>
-          <t>Shrewsbury</t>
+          <t>Cheltenham</t>
         </is>
       </c>
       <c r="I163" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J163" t="n">
-        <v>1.58</v>
+        <v>1.41</v>
       </c>
       <c r="K163" t="inlineStr">
         <is>
@@ -15408,15 +15408,15 @@
         </is>
       </c>
       <c r="L163" t="n">
-        <v>1.74</v>
+        <v>1.38</v>
       </c>
       <c r="M163" t="inlineStr">
         <is>
-          <t>24/10/2023 20:16</t>
+          <t>24/10/2023 20:36</t>
         </is>
       </c>
       <c r="N163" t="n">
-        <v>4.09</v>
+        <v>4.5</v>
       </c>
       <c r="O163" t="inlineStr">
         <is>
@@ -15424,15 +15424,15 @@
         </is>
       </c>
       <c r="P163" t="n">
-        <v>3.71</v>
+        <v>4.82</v>
       </c>
       <c r="Q163" t="inlineStr">
         <is>
-          <t>24/10/2023 20:37</t>
+          <t>24/10/2023 20:41</t>
         </is>
       </c>
       <c r="R163" t="n">
-        <v>5.9</v>
+        <v>7.23</v>
       </c>
       <c r="S163" t="inlineStr">
         <is>
@@ -15440,16 +15440,16 @@
         </is>
       </c>
       <c r="T163" t="n">
-        <v>5.2</v>
+        <v>9.26</v>
       </c>
       <c r="U163" t="inlineStr">
         <is>
-          <t>24/10/2023 20:43</t>
+          <t>24/10/2023 20:41</t>
         </is>
       </c>
       <c r="V163" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/barnsley-shrewsbury/zqQhGdUo/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/blackpool-cheltenham/EZOdFGqh/</t>
         </is>
       </c>
     </row>
@@ -15477,22 +15477,22 @@
       </c>
       <c r="F164" t="inlineStr">
         <is>
-          <t>Carlisle</t>
+          <t>Barnsley</t>
         </is>
       </c>
       <c r="G164" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H164" t="inlineStr">
         <is>
-          <t>Burton</t>
+          <t>Shrewsbury</t>
         </is>
       </c>
       <c r="I164" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J164" t="n">
-        <v>2.1</v>
+        <v>1.58</v>
       </c>
       <c r="K164" t="inlineStr">
         <is>
@@ -15500,15 +15500,15 @@
         </is>
       </c>
       <c r="L164" t="n">
-        <v>2.46</v>
+        <v>1.74</v>
       </c>
       <c r="M164" t="inlineStr">
         <is>
-          <t>24/10/2023 20:41</t>
+          <t>24/10/2023 20:16</t>
         </is>
       </c>
       <c r="N164" t="n">
-        <v>3.29</v>
+        <v>4.09</v>
       </c>
       <c r="O164" t="inlineStr">
         <is>
@@ -15516,15 +15516,15 @@
         </is>
       </c>
       <c r="P164" t="n">
-        <v>3.3</v>
+        <v>3.71</v>
       </c>
       <c r="Q164" t="inlineStr">
         <is>
-          <t>24/10/2023 20:41</t>
+          <t>24/10/2023 20:37</t>
         </is>
       </c>
       <c r="R164" t="n">
-        <v>3.57</v>
+        <v>5.9</v>
       </c>
       <c r="S164" t="inlineStr">
         <is>
@@ -15532,16 +15532,16 @@
         </is>
       </c>
       <c r="T164" t="n">
-        <v>3.09</v>
+        <v>5.2</v>
       </c>
       <c r="U164" t="inlineStr">
         <is>
-          <t>24/10/2023 20:41</t>
+          <t>24/10/2023 20:43</t>
         </is>
       </c>
       <c r="V164" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/carlisle-burton/Sbv2CETA/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/barnsley-shrewsbury/zqQhGdUo/</t>
         </is>
       </c>
     </row>
@@ -15661,22 +15661,22 @@
       </c>
       <c r="F166" t="inlineStr">
         <is>
-          <t>Wigan</t>
+          <t>Stevenage</t>
         </is>
       </c>
       <c r="G166" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H166" t="inlineStr">
         <is>
-          <t>Shrewsbury</t>
+          <t>Derby</t>
         </is>
       </c>
       <c r="I166" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J166" t="n">
-        <v>1.88</v>
+        <v>2.55</v>
       </c>
       <c r="K166" t="inlineStr">
         <is>
@@ -15684,15 +15684,15 @@
         </is>
       </c>
       <c r="L166" t="n">
-        <v>2.17</v>
+        <v>2.93</v>
       </c>
       <c r="M166" t="inlineStr">
         <is>
-          <t>28/10/2023 15:57</t>
+          <t>28/10/2023 15:44</t>
         </is>
       </c>
       <c r="N166" t="n">
-        <v>3.55</v>
+        <v>3.24</v>
       </c>
       <c r="O166" t="inlineStr">
         <is>
@@ -15700,15 +15700,15 @@
         </is>
       </c>
       <c r="P166" t="n">
-        <v>3.32</v>
+        <v>3.21</v>
       </c>
       <c r="Q166" t="inlineStr">
         <is>
-          <t>28/10/2023 15:57</t>
+          <t>28/10/2023 15:44</t>
         </is>
       </c>
       <c r="R166" t="n">
-        <v>4.34</v>
+        <v>2.93</v>
       </c>
       <c r="S166" t="inlineStr">
         <is>
@@ -15716,16 +15716,16 @@
         </is>
       </c>
       <c r="T166" t="n">
-        <v>3.69</v>
+        <v>2.64</v>
       </c>
       <c r="U166" t="inlineStr">
         <is>
-          <t>28/10/2023 15:57</t>
+          <t>28/10/2023 15:44</t>
         </is>
       </c>
       <c r="V166" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/wigan-shrewsbury/YyeM9XUQ/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/stevenage-derby/KYjIADFK/</t>
         </is>
       </c>
     </row>
@@ -15753,22 +15753,22 @@
       </c>
       <c r="F167" t="inlineStr">
         <is>
-          <t>Stevenage</t>
+          <t>Reading</t>
         </is>
       </c>
       <c r="G167" t="n">
+        <v>2</v>
+      </c>
+      <c r="H167" t="inlineStr">
+        <is>
+          <t>Portsmouth</t>
+        </is>
+      </c>
+      <c r="I167" t="n">
         <v>3</v>
       </c>
-      <c r="H167" t="inlineStr">
-        <is>
-          <t>Derby</t>
-        </is>
-      </c>
-      <c r="I167" t="n">
-        <v>1</v>
-      </c>
       <c r="J167" t="n">
-        <v>2.55</v>
+        <v>3.38</v>
       </c>
       <c r="K167" t="inlineStr">
         <is>
@@ -15776,15 +15776,15 @@
         </is>
       </c>
       <c r="L167" t="n">
-        <v>2.93</v>
+        <v>3.56</v>
       </c>
       <c r="M167" t="inlineStr">
         <is>
-          <t>28/10/2023 15:44</t>
+          <t>28/10/2023 15:56</t>
         </is>
       </c>
       <c r="N167" t="n">
-        <v>3.24</v>
+        <v>3.5</v>
       </c>
       <c r="O167" t="inlineStr">
         <is>
@@ -15792,15 +15792,15 @@
         </is>
       </c>
       <c r="P167" t="n">
-        <v>3.21</v>
+        <v>3.57</v>
       </c>
       <c r="Q167" t="inlineStr">
         <is>
-          <t>28/10/2023 15:44</t>
+          <t>28/10/2023 15:56</t>
         </is>
       </c>
       <c r="R167" t="n">
-        <v>2.93</v>
+        <v>2.08</v>
       </c>
       <c r="S167" t="inlineStr">
         <is>
@@ -15808,16 +15808,16 @@
         </is>
       </c>
       <c r="T167" t="n">
-        <v>2.64</v>
+        <v>2.11</v>
       </c>
       <c r="U167" t="inlineStr">
         <is>
-          <t>28/10/2023 15:44</t>
+          <t>28/10/2023 15:56</t>
         </is>
       </c>
       <c r="V167" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/stevenage-derby/KYjIADFK/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/reading-portsmouth/xA1DBg0E/</t>
         </is>
       </c>
     </row>
@@ -15845,7 +15845,7 @@
       </c>
       <c r="F168" t="inlineStr">
         <is>
-          <t>Reading</t>
+          <t>Wigan</t>
         </is>
       </c>
       <c r="G168" t="n">
@@ -15853,14 +15853,14 @@
       </c>
       <c r="H168" t="inlineStr">
         <is>
-          <t>Portsmouth</t>
+          <t>Shrewsbury</t>
         </is>
       </c>
       <c r="I168" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J168" t="n">
-        <v>3.38</v>
+        <v>1.88</v>
       </c>
       <c r="K168" t="inlineStr">
         <is>
@@ -15868,15 +15868,15 @@
         </is>
       </c>
       <c r="L168" t="n">
-        <v>3.56</v>
+        <v>2.17</v>
       </c>
       <c r="M168" t="inlineStr">
         <is>
-          <t>28/10/2023 15:56</t>
+          <t>28/10/2023 15:57</t>
         </is>
       </c>
       <c r="N168" t="n">
-        <v>3.5</v>
+        <v>3.55</v>
       </c>
       <c r="O168" t="inlineStr">
         <is>
@@ -15884,15 +15884,15 @@
         </is>
       </c>
       <c r="P168" t="n">
-        <v>3.57</v>
+        <v>3.32</v>
       </c>
       <c r="Q168" t="inlineStr">
         <is>
-          <t>28/10/2023 15:56</t>
+          <t>28/10/2023 15:57</t>
         </is>
       </c>
       <c r="R168" t="n">
-        <v>2.08</v>
+        <v>4.34</v>
       </c>
       <c r="S168" t="inlineStr">
         <is>
@@ -15900,16 +15900,16 @@
         </is>
       </c>
       <c r="T168" t="n">
-        <v>2.11</v>
+        <v>3.69</v>
       </c>
       <c r="U168" t="inlineStr">
         <is>
-          <t>28/10/2023 15:56</t>
+          <t>28/10/2023 15:57</t>
         </is>
       </c>
       <c r="V168" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/reading-portsmouth/xA1DBg0E/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/wigan-shrewsbury/YyeM9XUQ/</t>
         </is>
       </c>
     </row>
@@ -15937,22 +15937,22 @@
       </c>
       <c r="F169" t="inlineStr">
         <is>
-          <t>Port Vale</t>
+          <t>Oxford Utd</t>
         </is>
       </c>
       <c r="G169" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H169" t="inlineStr">
         <is>
-          <t>Cheltenham</t>
+          <t>Wycombe</t>
         </is>
       </c>
       <c r="I169" t="n">
         <v>2</v>
       </c>
       <c r="J169" t="n">
-        <v>1.75</v>
+        <v>1.71</v>
       </c>
       <c r="K169" t="inlineStr">
         <is>
@@ -15960,15 +15960,15 @@
         </is>
       </c>
       <c r="L169" t="n">
-        <v>1.74</v>
+        <v>1.93</v>
       </c>
       <c r="M169" t="inlineStr">
         <is>
-          <t>28/10/2023 15:55</t>
+          <t>28/10/2023 15:32</t>
         </is>
       </c>
       <c r="N169" t="n">
-        <v>3.63</v>
+        <v>3.88</v>
       </c>
       <c r="O169" t="inlineStr">
         <is>
@@ -15976,15 +15976,15 @@
         </is>
       </c>
       <c r="P169" t="n">
-        <v>3.79</v>
+        <v>3.59</v>
       </c>
       <c r="Q169" t="inlineStr">
         <is>
-          <t>28/10/2023 15:55</t>
+          <t>28/10/2023 15:59</t>
         </is>
       </c>
       <c r="R169" t="n">
-        <v>4.58</v>
+        <v>4.91</v>
       </c>
       <c r="S169" t="inlineStr">
         <is>
@@ -15992,16 +15992,16 @@
         </is>
       </c>
       <c r="T169" t="n">
-        <v>5.1</v>
+        <v>4.07</v>
       </c>
       <c r="U169" t="inlineStr">
         <is>
-          <t>28/10/2023 15:55</t>
+          <t>28/10/2023 15:59</t>
         </is>
       </c>
       <c r="V169" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/port-vale-cheltenham/bJ29CZp8/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/oxford-utd-wycombe/p2aSmj87/</t>
         </is>
       </c>
     </row>
@@ -16121,22 +16121,22 @@
       </c>
       <c r="F171" t="inlineStr">
         <is>
-          <t>Oxford Utd</t>
+          <t>Port Vale</t>
         </is>
       </c>
       <c r="G171" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H171" t="inlineStr">
         <is>
-          <t>Wycombe</t>
+          <t>Cheltenham</t>
         </is>
       </c>
       <c r="I171" t="n">
         <v>2</v>
       </c>
       <c r="J171" t="n">
-        <v>1.71</v>
+        <v>1.75</v>
       </c>
       <c r="K171" t="inlineStr">
         <is>
@@ -16144,15 +16144,15 @@
         </is>
       </c>
       <c r="L171" t="n">
-        <v>1.93</v>
+        <v>1.74</v>
       </c>
       <c r="M171" t="inlineStr">
         <is>
-          <t>28/10/2023 15:32</t>
+          <t>28/10/2023 15:55</t>
         </is>
       </c>
       <c r="N171" t="n">
-        <v>3.88</v>
+        <v>3.63</v>
       </c>
       <c r="O171" t="inlineStr">
         <is>
@@ -16160,15 +16160,15 @@
         </is>
       </c>
       <c r="P171" t="n">
-        <v>3.59</v>
+        <v>3.79</v>
       </c>
       <c r="Q171" t="inlineStr">
         <is>
-          <t>28/10/2023 15:59</t>
+          <t>28/10/2023 15:55</t>
         </is>
       </c>
       <c r="R171" t="n">
-        <v>4.91</v>
+        <v>4.58</v>
       </c>
       <c r="S171" t="inlineStr">
         <is>
@@ -16176,16 +16176,16 @@
         </is>
       </c>
       <c r="T171" t="n">
-        <v>4.07</v>
+        <v>5.1</v>
       </c>
       <c r="U171" t="inlineStr">
         <is>
-          <t>28/10/2023 15:59</t>
+          <t>28/10/2023 15:55</t>
         </is>
       </c>
       <c r="V171" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/england/league-one/oxford-utd-wycombe/p2aSmj87/</t>
+          <t>https://www.betexplorer.com/football/england/league-one/port-vale-cheltenham/bJ29CZp8/</t>
         </is>
       </c>
     </row>
@@ -18762,6 +18762,98 @@
       <c r="V199" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/england/league-one/stevenage-lincoln-city/YLzFSoy6/</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" s="1" t="n">
+        <v>199</v>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>england</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>league-one</t>
+        </is>
+      </c>
+      <c r="D200" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E200" s="2" t="n">
+        <v>45251.86458333334</v>
+      </c>
+      <c r="F200" t="inlineStr">
+        <is>
+          <t>Leyton Orient</t>
+        </is>
+      </c>
+      <c r="G200" t="n">
+        <v>0</v>
+      </c>
+      <c r="H200" t="inlineStr">
+        <is>
+          <t>Lincoln</t>
+        </is>
+      </c>
+      <c r="I200" t="n">
+        <v>1</v>
+      </c>
+      <c r="J200" t="n">
+        <v>2.49</v>
+      </c>
+      <c r="K200" t="inlineStr">
+        <is>
+          <t>30/09/2023 23:42</t>
+        </is>
+      </c>
+      <c r="L200" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="M200" t="inlineStr">
+        <is>
+          <t>21/11/2023 20:30</t>
+        </is>
+      </c>
+      <c r="N200" t="n">
+        <v>3.16</v>
+      </c>
+      <c r="O200" t="inlineStr">
+        <is>
+          <t>30/09/2023 23:42</t>
+        </is>
+      </c>
+      <c r="P200" t="n">
+        <v>3.38</v>
+      </c>
+      <c r="Q200" t="inlineStr">
+        <is>
+          <t>21/11/2023 20:30</t>
+        </is>
+      </c>
+      <c r="R200" t="n">
+        <v>2.92</v>
+      </c>
+      <c r="S200" t="inlineStr">
+        <is>
+          <t>30/09/2023 23:42</t>
+        </is>
+      </c>
+      <c r="T200" t="n">
+        <v>4.68</v>
+      </c>
+      <c r="U200" t="inlineStr">
+        <is>
+          <t>21/11/2023 20:30</t>
+        </is>
+      </c>
+      <c r="V200" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/england/league-one/leyton-orient-lincoln-city/t6fmrCI2/</t>
         </is>
       </c>
     </row>

</xml_diff>